<commit_message>
query for vars in group working!
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen.Sheppard\PycharmProjects\PneumoCaT2\Database_tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea2a525dac66033e/Documents/PneumoCaT2/Database_tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_125CC56CC83245DB58EB9C0A768C8C7818829FB8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6510" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Serotype" sheetId="1" r:id="rId1"/>
@@ -727,7 +728,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1163,23 +1164,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="17" width="9.140625" style="2"/>
-    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="3"/>
+    <col min="4" max="17" width="9.1328125" style="2"/>
+    <col min="18" max="18" width="11.86328125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>196</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>192</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>198</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>223</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>224</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>222</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>42</v>
       </c>
@@ -1514,7 +1515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>50</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>60</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>61</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>65</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>67</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>68</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>69</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>70</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>71</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>74</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>75</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>77</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>79</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>80</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>81</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>83</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>85</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="6" t="s">
         <v>86</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>88</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>89</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="6" t="s">
         <v>91</v>
       </c>
@@ -2026,7 +2027,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>92</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>93</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="6" t="s">
         <v>94</v>
       </c>
@@ -2059,7 +2060,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="6" t="s">
         <v>95</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>96</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="6" t="s">
         <v>97</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
         <v>99</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>100</v>
       </c>
@@ -2141,9 +2142,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>105</v>
@@ -2167,7 +2168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="6" t="s">
         <v>106</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="6" t="s">
         <v>111</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="6" t="s">
         <v>112</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
         <v>113</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="6" t="s">
         <v>114</v>
       </c>
@@ -2234,7 +2235,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="6" t="s">
         <v>115</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="6" t="s">
         <v>116</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="6" t="s">
         <v>117</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="6" t="s">
         <v>118</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="6" t="s">
         <v>120</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="6" t="s">
         <v>121</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="6" t="s">
         <v>124</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="6" t="s">
         <v>125</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="6" t="s">
         <v>126</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="6" t="s">
         <v>128</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="6" t="s">
         <v>129</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="6" t="s">
         <v>132</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="6" t="s">
         <v>133</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="6" t="s">
         <v>134</v>
       </c>
@@ -2426,7 +2427,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="6" t="s">
         <v>137</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="6" t="s">
         <v>138</v>
       </c>
@@ -2460,7 +2461,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="6" t="s">
         <v>140</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="6" t="s">
         <v>141</v>
       </c>
@@ -2482,7 +2483,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="6" t="s">
         <v>142</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="6" t="s">
         <v>143</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="6" t="s">
         <v>144</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="6" t="s">
         <v>146</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="6" t="s">
         <v>147</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="6" t="s">
         <v>148</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="6" t="s">
         <v>149</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="6" t="s">
         <v>151</v>
       </c>
@@ -2603,7 +2604,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="6" t="s">
         <v>152</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="6" t="s">
         <v>153</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="6" t="s">
         <v>154</v>
       </c>
@@ -2636,7 +2637,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="6" t="s">
         <v>225</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="6" t="s">
         <v>50</v>
       </c>
@@ -2658,7 +2659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="6" t="s">
         <v>155</v>
       </c>
@@ -2669,7 +2670,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="6" t="s">
         <v>156</v>
       </c>
@@ -2680,7 +2681,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="6" t="s">
         <v>157</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="6" t="s">
         <v>158</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="6" t="s">
         <v>159</v>
       </c>
@@ -2713,7 +2714,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="6" t="s">
         <v>160</v>
       </c>
@@ -2724,7 +2725,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="6" t="s">
         <v>161</v>
       </c>
@@ -2742,103 +2743,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="G182" sqref="G182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.265625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.265625" style="1" customWidth="1"/>
     <col min="19" max="19" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.28515625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="22.265625" style="1" customWidth="1"/>
     <col min="29" max="29" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="22.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="9.140625" style="1"/>
+    <col min="85" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>196</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -2931,7 +2932,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -2948,7 +2949,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -2993,7 +2994,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
@@ -3041,7 +3042,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -3058,7 +3059,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
@@ -3137,7 +3138,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>61</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>61</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -3341,7 +3342,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -3358,7 +3359,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -3392,7 +3393,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
@@ -3460,7 +3461,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -3520,7 +3521,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>77</v>
       </c>
@@ -3554,7 +3555,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
@@ -3571,7 +3572,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>77</v>
       </c>
@@ -3588,7 +3589,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>77</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>77</v>
       </c>
@@ -3622,7 +3623,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>77</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>77</v>
       </c>
@@ -3656,7 +3657,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
@@ -3673,7 +3674,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>77</v>
       </c>
@@ -3690,7 +3691,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>77</v>
       </c>
@@ -3724,7 +3725,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>77</v>
       </c>
@@ -3758,7 +3759,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>78</v>
       </c>
@@ -3773,7 +3774,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>78</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>78</v>
       </c>
@@ -3824,7 +3825,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>78</v>
       </c>
@@ -3841,7 +3842,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>78</v>
       </c>
@@ -3858,7 +3859,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>78</v>
       </c>
@@ -3875,7 +3876,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>78</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
@@ -3909,7 +3910,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>78</v>
       </c>
@@ -3926,7 +3927,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
@@ -3943,7 +3944,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>78</v>
       </c>
@@ -3960,7 +3961,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>78</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>78</v>
       </c>
@@ -3994,7 +3995,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>78</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>79</v>
       </c>
@@ -4026,7 +4027,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>79</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
@@ -4060,7 +4061,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>79</v>
       </c>
@@ -4077,7 +4078,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>79</v>
       </c>
@@ -4094,7 +4095,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>79</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>79</v>
       </c>
@@ -4128,7 +4129,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>79</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>79</v>
       </c>
@@ -4179,7 +4180,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" s="3" t="s">
         <v>79</v>
       </c>
@@ -4196,7 +4197,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
@@ -4213,7 +4214,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>79</v>
       </c>
@@ -4230,7 +4231,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>79</v>
       </c>
@@ -4247,7 +4248,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>79</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>80</v>
       </c>
@@ -4278,7 +4279,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>80</v>
       </c>
@@ -4295,7 +4296,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>80</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>80</v>
       </c>
@@ -4329,7 +4330,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>80</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>80</v>
       </c>
@@ -4363,7 +4364,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>80</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>80</v>
       </c>
@@ -4397,7 +4398,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>80</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>80</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>80</v>
       </c>
@@ -4448,7 +4449,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>80</v>
       </c>
@@ -4465,7 +4466,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>80</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>80</v>
       </c>
@@ -4499,7 +4500,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>80</v>
       </c>
@@ -4516,7 +4517,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>81</v>
       </c>
@@ -4530,7 +4531,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>81</v>
       </c>
@@ -4547,7 +4548,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>81</v>
       </c>
@@ -4564,7 +4565,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>81</v>
       </c>
@@ -4581,7 +4582,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>81</v>
       </c>
@@ -4598,7 +4599,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>81</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>81</v>
       </c>
@@ -4632,7 +4633,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>81</v>
       </c>
@@ -4649,7 +4650,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>81</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>81</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>81</v>
       </c>
@@ -4700,7 +4701,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>81</v>
       </c>
@@ -4717,7 +4718,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>81</v>
       </c>
@@ -4734,7 +4735,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>81</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116" s="3" t="s">
         <v>81</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>85</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>85</v>
       </c>
@@ -4796,7 +4797,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>85</v>
       </c>
@@ -4810,7 +4811,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>85</v>
       </c>
@@ -4824,7 +4825,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>86</v>
       </c>
@@ -4838,7 +4839,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>86</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>86</v>
       </c>
@@ -4866,7 +4867,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>86</v>
       </c>
@@ -4880,7 +4881,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>88</v>
       </c>
@@ -4894,7 +4895,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>89</v>
       </c>
@@ -4908,7 +4909,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>96</v>
       </c>
@@ -4922,7 +4923,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>97</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>100</v>
       </c>
@@ -4950,7 +4951,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>106</v>
       </c>
@@ -4964,7 +4965,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>128</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>128</v>
       </c>
@@ -4998,7 +4999,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>128</v>
       </c>
@@ -5015,7 +5016,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>128</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>128</v>
       </c>
@@ -5049,7 +5050,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>128</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>128</v>
       </c>
@@ -5083,7 +5084,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>128</v>
       </c>
@@ -5100,7 +5101,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>128</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>128</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>128</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>128</v>
       </c>
@@ -5168,7 +5169,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>128</v>
       </c>
@@ -5185,7 +5186,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>128</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>128</v>
       </c>
@@ -5219,7 +5220,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>128</v>
       </c>
@@ -5236,7 +5237,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>128</v>
       </c>
@@ -5253,7 +5254,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>128</v>
       </c>
@@ -5270,7 +5271,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>128</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>129</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>129</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>129</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>129</v>
       </c>
@@ -5355,7 +5356,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>129</v>
       </c>
@@ -5372,7 +5373,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>129</v>
       </c>
@@ -5389,7 +5390,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="3" t="s">
         <v>129</v>
       </c>
@@ -5406,7 +5407,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>129</v>
       </c>
@@ -5423,7 +5424,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>129</v>
       </c>
@@ -5440,7 +5441,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>129</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="3" t="s">
         <v>129</v>
       </c>
@@ -5474,7 +5475,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="3" t="s">
         <v>129</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="3" t="s">
         <v>129</v>
       </c>
@@ -5508,7 +5509,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="3" t="s">
         <v>129</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="3" t="s">
         <v>129</v>
       </c>
@@ -5542,7 +5543,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A165" s="3" t="s">
         <v>129</v>
       </c>
@@ -5559,7 +5560,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A166" s="3" t="s">
         <v>129</v>
       </c>
@@ -5576,7 +5577,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A167" s="3" t="s">
         <v>129</v>
       </c>
@@ -5593,7 +5594,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A168" s="3" t="s">
         <v>129</v>
       </c>
@@ -5610,7 +5611,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A169" s="3" t="s">
         <v>137</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A170" s="3" t="s">
         <v>138</v>
       </c>
@@ -5638,7 +5639,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A171" s="3" t="s">
         <v>144</v>
       </c>
@@ -5652,7 +5653,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A172" s="3" t="s">
         <v>146</v>
       </c>
@@ -5666,7 +5667,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A173" s="3" t="s">
         <v>147</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A174" s="3" t="s">
         <v>147</v>
       </c>
@@ -5697,7 +5698,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A175" s="3" t="s">
         <v>147</v>
       </c>
@@ -5714,7 +5715,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A176" s="3" t="s">
         <v>147</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A177" s="3" t="s">
         <v>147</v>
       </c>
@@ -5748,7 +5749,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A178" s="3" t="s">
         <v>147</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A179" s="3" t="s">
         <v>147</v>
       </c>
@@ -5782,7 +5783,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A180" s="3" t="s">
         <v>147</v>
       </c>
@@ -5799,7 +5800,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A181" s="3" t="s">
         <v>147</v>
       </c>
@@ -5816,7 +5817,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A182" s="3" t="s">
         <v>147</v>
       </c>
@@ -5833,7 +5834,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A183" s="3" t="s">
         <v>147</v>
       </c>
@@ -5850,7 +5851,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A184" s="3" t="s">
         <v>147</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A185" s="3" t="s">
         <v>148</v>
       </c>
@@ -5881,7 +5882,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A186" s="3" t="s">
         <v>148</v>
       </c>
@@ -5898,7 +5899,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A187" s="3" t="s">
         <v>148</v>
       </c>
@@ -5915,7 +5916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A188" s="3" t="s">
         <v>148</v>
       </c>
@@ -5932,7 +5933,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A189" s="3" t="s">
         <v>148</v>
       </c>
@@ -5949,7 +5950,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A190" s="3" t="s">
         <v>148</v>
       </c>
@@ -5966,7 +5967,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A191" s="3" t="s">
         <v>148</v>
       </c>
@@ -5983,7 +5984,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A192" s="3" t="s">
         <v>148</v>
       </c>
@@ -6000,7 +6001,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A193" s="3" t="s">
         <v>148</v>
       </c>
@@ -6017,7 +6018,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194" s="3" t="s">
         <v>148</v>
       </c>
@@ -6034,7 +6035,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A195" s="3" t="s">
         <v>148</v>
       </c>
@@ -6051,7 +6052,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A196" s="3" t="s">
         <v>148</v>
       </c>
@@ -6068,7 +6069,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A197" s="3" t="s">
         <v>149</v>
       </c>
@@ -6082,7 +6083,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198" s="3" t="s">
         <v>149</v>
       </c>
@@ -6099,7 +6100,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A199" s="3" t="s">
         <v>149</v>
       </c>
@@ -6116,7 +6117,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A200" s="3" t="s">
         <v>149</v>
       </c>
@@ -6133,7 +6134,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A201" s="3" t="s">
         <v>149</v>
       </c>
@@ -6150,7 +6151,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A202" s="3" t="s">
         <v>149</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A203" s="3" t="s">
         <v>149</v>
       </c>
@@ -6184,7 +6185,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A204" s="3" t="s">
         <v>149</v>
       </c>
@@ -6201,7 +6202,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A205" s="3" t="s">
         <v>149</v>
       </c>
@@ -6218,7 +6219,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A206" s="3" t="s">
         <v>149</v>
       </c>
@@ -6235,7 +6236,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A207" s="3" t="s">
         <v>149</v>
       </c>
@@ -6252,7 +6253,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A208" s="3" t="s">
         <v>149</v>
       </c>
@@ -6270,9 +6271,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E208"/>
+  <autoFilter ref="A1:E208" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6282,99 +6283,99 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>150</v>
       </c>
@@ -6385,30 +6386,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E19" sqref="A19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" style="9" customWidth="1"/>
     <col min="2" max="2" width="20" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="14"/>
+    <col min="3" max="3" width="9.1328125" style="14"/>
     <col min="4" max="4" width="14" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
-    <col min="10" max="13" width="11.28515625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="18.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="18.73046875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.265625" style="3" customWidth="1"/>
+    <col min="10" max="13" width="11.265625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.1328125" style="3"/>
+    <col min="15" max="15" width="18.3984375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>163</v>
       </c>
@@ -6427,7 +6428,7 @@
       <c r="G1"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>166</v>
       </c>
@@ -6443,7 +6444,7 @@
       <c r="G2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>166</v>
       </c>
@@ -6459,7 +6460,7 @@
       <c r="G3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>166</v>
       </c>
@@ -6475,7 +6476,7 @@
       <c r="G4"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>166</v>
       </c>
@@ -6491,7 +6492,7 @@
       <c r="G5"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>166</v>
       </c>
@@ -6507,7 +6508,7 @@
       <c r="G6"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>166</v>
       </c>
@@ -6523,7 +6524,7 @@
       <c r="G7"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>166</v>
       </c>
@@ -6539,7 +6540,7 @@
       <c r="G8"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>168</v>
       </c>
@@ -6555,7 +6556,7 @@
       <c r="G9"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>168</v>
       </c>
@@ -6571,7 +6572,7 @@
       <c r="G10"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>168</v>
       </c>
@@ -6587,7 +6588,7 @@
       <c r="G11"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>168</v>
       </c>
@@ -6603,7 +6604,7 @@
       <c r="G12"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>168</v>
       </c>
@@ -6619,7 +6620,7 @@
       <c r="G13"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>168</v>
       </c>
@@ -6635,7 +6636,7 @@
       <c r="G14"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>168</v>
       </c>
@@ -6651,7 +6652,7 @@
       <c r="G15"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>168</v>
       </c>
@@ -6667,7 +6668,7 @@
       <c r="G16"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>168</v>
       </c>
@@ -6683,7 +6684,7 @@
       <c r="G17"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>168</v>
       </c>
@@ -6699,7 +6700,7 @@
       <c r="G18"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>168</v>
       </c>
@@ -6715,7 +6716,7 @@
       <c r="G19"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>168</v>
       </c>
@@ -6731,7 +6732,7 @@
       <c r="G20"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>168</v>
       </c>
@@ -6747,7 +6748,7 @@
       <c r="G21"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>168</v>
       </c>
@@ -6763,7 +6764,7 @@
       <c r="G22"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>168</v>
       </c>
@@ -6779,7 +6780,7 @@
       <c r="G23"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>168</v>
       </c>
@@ -6795,7 +6796,7 @@
       <c r="G24"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>175</v>
       </c>
@@ -6811,7 +6812,7 @@
       <c r="G25"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>175</v>
       </c>
@@ -6827,7 +6828,7 @@
       <c r="G26"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>175</v>
       </c>
@@ -6843,7 +6844,7 @@
       <c r="G27"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>175</v>
       </c>
@@ -6859,7 +6860,7 @@
       <c r="G28"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>175</v>
       </c>
@@ -6875,7 +6876,7 @@
       <c r="G29"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>175</v>
       </c>
@@ -6891,7 +6892,7 @@
       <c r="G30"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>175</v>
       </c>
@@ -6907,7 +6908,7 @@
       <c r="G31"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>175</v>
       </c>
@@ -6923,7 +6924,7 @@
       <c r="G32"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>179</v>
       </c>
@@ -6942,7 +6943,7 @@
       <c r="G33"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>179</v>
       </c>
@@ -6961,7 +6962,7 @@
       <c r="G34"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>179</v>
       </c>
@@ -6980,7 +6981,7 @@
       <c r="G35"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>179</v>
       </c>
@@ -6999,7 +7000,7 @@
       <c r="G36"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>179</v>
       </c>
@@ -7018,7 +7019,7 @@
       <c r="G37"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>179</v>
       </c>
@@ -7037,7 +7038,7 @@
       <c r="G38"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>179</v>
       </c>
@@ -7056,7 +7057,7 @@
       <c r="G39"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>179</v>
       </c>
@@ -7075,7 +7076,7 @@
       <c r="G40"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>179</v>
       </c>
@@ -7094,7 +7095,7 @@
       <c r="G41"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>179</v>
       </c>
@@ -7113,7 +7114,7 @@
       <c r="G42"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>179</v>
       </c>
@@ -7132,7 +7133,7 @@
       <c r="G43"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>179</v>
       </c>
@@ -7151,7 +7152,7 @@
       <c r="G44"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>179</v>
       </c>
@@ -7170,7 +7171,7 @@
       <c r="G45"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>179</v>
       </c>
@@ -7189,7 +7190,7 @@
       <c r="G46"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>179</v>
       </c>
@@ -7208,7 +7209,7 @@
       <c r="G47"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>179</v>
       </c>
@@ -7227,7 +7228,7 @@
       <c r="G48"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>179</v>
       </c>
@@ -7246,7 +7247,7 @@
       <c r="G49"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>179</v>
       </c>
@@ -7265,7 +7266,7 @@
       <c r="G50"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>179</v>
       </c>
@@ -7284,7 +7285,7 @@
       <c r="G51"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>179</v>
       </c>
@@ -7303,7 +7304,7 @@
       <c r="G52"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -7322,7 +7323,7 @@
       <c r="G53"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>179</v>
       </c>
@@ -7341,7 +7342,7 @@
       <c r="G54"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>179</v>
       </c>
@@ -7360,7 +7361,7 @@
       <c r="G55"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>179</v>
       </c>
@@ -7379,7 +7380,7 @@
       <c r="G56"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>179</v>
       </c>
@@ -7398,7 +7399,7 @@
       <c r="G57"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>179</v>
       </c>
@@ -7417,7 +7418,7 @@
       <c r="G58"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>179</v>
       </c>
@@ -7436,7 +7437,7 @@
       <c r="G59"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>179</v>
       </c>
@@ -7455,7 +7456,7 @@
       <c r="G60"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>179</v>
       </c>
@@ -7474,7 +7475,7 @@
       <c r="G61"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="9" t="s">
         <v>179</v>
       </c>
@@ -7493,7 +7494,7 @@
       <c r="G62"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="9" t="s">
         <v>179</v>
       </c>
@@ -7512,7 +7513,7 @@
       <c r="G63"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>179</v>
       </c>
@@ -7531,7 +7532,7 @@
       <c r="G64"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="9" t="s">
         <v>179</v>
       </c>
@@ -7550,7 +7551,7 @@
       <c r="G65"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="9" t="s">
         <v>179</v>
       </c>
@@ -7569,7 +7570,7 @@
       <c r="G66"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="9" t="s">
         <v>179</v>
       </c>
@@ -7588,7 +7589,7 @@
       <c r="G67"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="9" t="s">
         <v>179</v>
       </c>
@@ -7607,7 +7608,7 @@
       <c r="G68"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="9" t="s">
         <v>179</v>
       </c>
@@ -7626,7 +7627,7 @@
       <c r="G69"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>179</v>
       </c>
@@ -7645,7 +7646,7 @@
       <c r="G70"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>179</v>
       </c>
@@ -7664,7 +7665,7 @@
       <c r="G71"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A72" s="9" t="s">
         <v>179</v>
       </c>
@@ -7683,7 +7684,7 @@
       <c r="G72"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A73" s="9" t="s">
         <v>179</v>
       </c>
@@ -7702,7 +7703,7 @@
       <c r="G73"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A74" s="9" t="s">
         <v>179</v>
       </c>
@@ -7721,7 +7722,7 @@
       <c r="G74"/>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A75" s="9" t="s">
         <v>179</v>
       </c>
@@ -7740,7 +7741,7 @@
       <c r="G75"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A76" s="9" t="s">
         <v>179</v>
       </c>
@@ -7759,7 +7760,7 @@
       <c r="G76"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A77" s="9" t="s">
         <v>179</v>
       </c>
@@ -7778,7 +7779,7 @@
       <c r="G77"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A78" s="9" t="s">
         <v>179</v>
       </c>
@@ -7797,7 +7798,7 @@
       <c r="G78"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A79" s="9" t="s">
         <v>179</v>
       </c>
@@ -7816,7 +7817,7 @@
       <c r="G79"/>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A80" s="9" t="s">
         <v>179</v>
       </c>
@@ -7835,7 +7836,7 @@
       <c r="G80"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A81" s="9" t="s">
         <v>179</v>
       </c>
@@ -7854,7 +7855,7 @@
       <c r="G81"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A82" s="9" t="s">
         <v>179</v>
       </c>
@@ -7873,7 +7874,7 @@
       <c r="G82"/>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A83" s="9" t="s">
         <v>179</v>
       </c>
@@ -7892,7 +7893,7 @@
       <c r="G83"/>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A84" s="9" t="s">
         <v>179</v>
       </c>
@@ -7911,7 +7912,7 @@
       <c r="G84"/>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A85" s="9" t="s">
         <v>179</v>
       </c>
@@ -7930,7 +7931,7 @@
       <c r="G85"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A86" s="9" t="s">
         <v>179</v>
       </c>
@@ -7948,7 +7949,7 @@
       </c>
       <c r="H86" s="3"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A87" s="9" t="s">
         <v>179</v>
       </c>
@@ -7966,7 +7967,7 @@
       </c>
       <c r="H87" s="3"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A88" s="9" t="s">
         <v>179</v>
       </c>
@@ -7984,7 +7985,7 @@
       </c>
       <c r="H88" s="3"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A89" s="9" t="s">
         <v>179</v>
       </c>
@@ -8002,7 +8003,7 @@
       </c>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A90" s="9" t="s">
         <v>179</v>
       </c>
@@ -8020,7 +8021,7 @@
       </c>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A91" s="9" t="s">
         <v>179</v>
       </c>
@@ -8038,7 +8039,7 @@
       </c>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A92" s="9" t="s">
         <v>179</v>
       </c>
@@ -8056,7 +8057,7 @@
       </c>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A93" s="9" t="s">
         <v>179</v>
       </c>
@@ -8074,7 +8075,7 @@
       </c>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A94" s="9" t="s">
         <v>179</v>
       </c>
@@ -8092,7 +8093,7 @@
       </c>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A95" s="9" t="s">
         <v>179</v>
       </c>
@@ -8110,7 +8111,7 @@
       </c>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A96" s="9" t="s">
         <v>179</v>
       </c>
@@ -8128,7 +8129,7 @@
       </c>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A97" s="9" t="s">
         <v>179</v>
       </c>
@@ -8146,7 +8147,7 @@
       </c>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A98" s="9" t="s">
         <v>179</v>
       </c>
@@ -8164,7 +8165,7 @@
       </c>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A99" s="9" t="s">
         <v>179</v>
       </c>
@@ -8182,7 +8183,7 @@
       </c>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A100" s="9" t="s">
         <v>179</v>
       </c>
@@ -8200,7 +8201,7 @@
       </c>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A101" s="9" t="s">
         <v>179</v>
       </c>
@@ -8218,7 +8219,7 @@
       </c>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A102" s="9" t="s">
         <v>179</v>
       </c>
@@ -8236,7 +8237,7 @@
       </c>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A103" s="9" t="s">
         <v>179</v>
       </c>
@@ -8254,7 +8255,7 @@
       </c>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A104" s="9" t="s">
         <v>179</v>
       </c>
@@ -8272,7 +8273,7 @@
       </c>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A105" s="9" t="s">
         <v>179</v>
       </c>
@@ -8290,7 +8291,7 @@
       </c>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A106" s="9" t="s">
         <v>179</v>
       </c>
@@ -8308,7 +8309,7 @@
       </c>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A107" s="9" t="s">
         <v>179</v>
       </c>
@@ -8326,7 +8327,7 @@
       </c>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A108" s="9" t="s">
         <v>179</v>
       </c>
@@ -8344,7 +8345,7 @@
       </c>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A109" s="9" t="s">
         <v>179</v>
       </c>
@@ -8362,7 +8363,7 @@
       </c>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A110" s="9" t="s">
         <v>179</v>
       </c>
@@ -8380,7 +8381,7 @@
       </c>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A111" s="9" t="s">
         <v>179</v>
       </c>
@@ -8398,7 +8399,7 @@
       </c>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A112" s="9" t="s">
         <v>179</v>
       </c>
@@ -8416,7 +8417,7 @@
       </c>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A113" s="9" t="s">
         <v>179</v>
       </c>
@@ -8434,7 +8435,7 @@
       </c>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A114" s="9" t="s">
         <v>179</v>
       </c>
@@ -8452,7 +8453,7 @@
       </c>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A115" s="9" t="s">
         <v>179</v>
       </c>
@@ -8470,7 +8471,7 @@
       </c>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A116" s="9" t="s">
         <v>179</v>
       </c>
@@ -8488,7 +8489,7 @@
       </c>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A117" s="9" t="s">
         <v>179</v>
       </c>
@@ -8506,7 +8507,7 @@
       </c>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A118" s="9" t="s">
         <v>179</v>
       </c>
@@ -8524,7 +8525,7 @@
       </c>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A119" s="9" t="s">
         <v>179</v>
       </c>
@@ -8542,7 +8543,7 @@
       </c>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A120" s="9" t="s">
         <v>179</v>
       </c>
@@ -8560,7 +8561,7 @@
       </c>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A121" s="9" t="s">
         <v>179</v>
       </c>
@@ -8578,7 +8579,7 @@
       </c>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A122" s="9" t="s">
         <v>179</v>
       </c>
@@ -8596,7 +8597,7 @@
       </c>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A123" s="9" t="s">
         <v>179</v>
       </c>
@@ -8614,7 +8615,7 @@
       </c>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A124" s="9" t="s">
         <v>179</v>
       </c>
@@ -8633,7 +8634,7 @@
       <c r="G124"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A125" s="9" t="s">
         <v>179</v>
       </c>
@@ -8652,7 +8653,7 @@
       <c r="G125"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A126" s="9" t="s">
         <v>179</v>
       </c>
@@ -8671,7 +8672,7 @@
       <c r="G126"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A127" s="9" t="s">
         <v>179</v>
       </c>
@@ -8690,7 +8691,7 @@
       <c r="G127"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A128" s="9" t="s">
         <v>179</v>
       </c>
@@ -8709,7 +8710,7 @@
       <c r="G128"/>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A129" s="9" t="s">
         <v>179</v>
       </c>
@@ -8728,7 +8729,7 @@
       <c r="G129"/>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A130" s="9" t="s">
         <v>179</v>
       </c>
@@ -8747,7 +8748,7 @@
       <c r="G130"/>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A131" s="9" t="s">
         <v>179</v>
       </c>
@@ -8766,7 +8767,7 @@
       <c r="G131"/>
       <c r="H131" s="3"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A132" s="9" t="s">
         <v>179</v>
       </c>
@@ -8785,7 +8786,7 @@
       <c r="G132"/>
       <c r="H132" s="3"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A133" s="9" t="s">
         <v>179</v>
       </c>
@@ -8804,7 +8805,7 @@
       <c r="G133"/>
       <c r="H133" s="3"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A134" s="9" t="s">
         <v>179</v>
       </c>
@@ -8823,7 +8824,7 @@
       <c r="G134"/>
       <c r="H134" s="3"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A135" s="9" t="s">
         <v>179</v>
       </c>
@@ -8842,7 +8843,7 @@
       <c r="G135"/>
       <c r="H135" s="3"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A136" s="9" t="s">
         <v>179</v>
       </c>
@@ -8861,7 +8862,7 @@
       <c r="G136"/>
       <c r="H136" s="3"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A137" s="9" t="s">
         <v>179</v>
       </c>
@@ -8880,7 +8881,7 @@
       <c r="G137"/>
       <c r="H137" s="3"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A138" s="9" t="s">
         <v>179</v>
       </c>
@@ -8899,7 +8900,7 @@
       <c r="G138"/>
       <c r="H138" s="3"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A139" s="9" t="s">
         <v>179</v>
       </c>
@@ -8918,7 +8919,7 @@
       <c r="G139"/>
       <c r="H139" s="3"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A140" s="9" t="s">
         <v>179</v>
       </c>
@@ -8937,7 +8938,7 @@
       <c r="G140"/>
       <c r="H140" s="3"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A141" s="9" t="s">
         <v>179</v>
       </c>
@@ -8956,7 +8957,7 @@
       <c r="G141"/>
       <c r="H141" s="3"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A142" s="9" t="s">
         <v>179</v>
       </c>
@@ -8975,7 +8976,7 @@
       <c r="G142"/>
       <c r="H142" s="3"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A143" s="9" t="s">
         <v>179</v>
       </c>
@@ -8994,7 +8995,7 @@
       <c r="G143"/>
       <c r="H143" s="3"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A144" s="9" t="s">
         <v>179</v>
       </c>
@@ -9013,7 +9014,7 @@
       <c r="G144"/>
       <c r="H144" s="3"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A145" s="9" t="s">
         <v>179</v>
       </c>
@@ -9032,7 +9033,7 @@
       <c r="G145"/>
       <c r="H145" s="3"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A146" s="9" t="s">
         <v>179</v>
       </c>
@@ -9051,7 +9052,7 @@
       <c r="G146"/>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A147" s="9" t="s">
         <v>179</v>
       </c>
@@ -9070,7 +9071,7 @@
       <c r="G147"/>
       <c r="H147" s="3"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A148" s="9" t="s">
         <v>179</v>
       </c>
@@ -9089,7 +9090,7 @@
       <c r="G148"/>
       <c r="H148" s="3"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A149" s="9" t="s">
         <v>179</v>
       </c>
@@ -9109,7 +9110,7 @@
       <c r="H149" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E149"/>
+  <autoFilter ref="A1:E149" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add catch for phenotype ctvdberror and fix upload template
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ea2a525dac66033e/Documents/PneumoCaT2/Database_tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen.Sheppard\Dropbox\WORK STUFF\PneumoCaT2\Database_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_125CC56CC83245DB58EB9C0A768C8C7818829FB8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="1. Serotype" sheetId="1" r:id="rId1"/>
@@ -728,7 +727,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1164,23 +1163,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.73046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="3"/>
-    <col min="4" max="17" width="9.1328125" style="2"/>
-    <col min="18" max="18" width="11.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="17" width="9.140625" style="2"/>
+    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>196</v>
       </c>
@@ -1236,7 +1235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>192</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>198</v>
       </c>
@@ -1258,7 +1257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>223</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>224</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>222</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1347,7 +1346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>42</v>
       </c>
@@ -1515,7 +1514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
@@ -1532,7 +1531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>47</v>
       </c>
@@ -1549,7 +1548,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
@@ -1566,7 +1565,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>50</v>
       </c>
@@ -1583,7 +1582,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -1594,7 +1593,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
@@ -1605,7 +1604,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -1622,7 +1621,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>60</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>61</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>65</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
@@ -1684,7 +1683,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>67</v>
       </c>
@@ -1695,7 +1694,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>68</v>
       </c>
@@ -1706,7 +1705,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>69</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>70</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>71</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>72</v>
       </c>
@@ -1762,7 +1761,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>74</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>75</v>
       </c>
@@ -1796,7 +1795,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>77</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
@@ -1848,7 +1847,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>79</v>
       </c>
@@ -1874,7 +1873,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>80</v>
       </c>
@@ -1900,7 +1899,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>81</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>83</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>85</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>86</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>88</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>89</v>
       </c>
@@ -2016,7 +2015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>91</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>92</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>93</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>94</v>
       </c>
@@ -2060,7 +2059,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>95</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>96</v>
       </c>
@@ -2088,7 +2087,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>97</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>99</v>
       </c>
@@ -2116,7 +2115,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>100</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>106</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>106</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>111</v>
       </c>
@@ -2202,7 +2201,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>112</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>113</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>114</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>115</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>116</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>117</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>118</v>
       </c>
@@ -2282,7 +2281,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>120</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>121</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>124</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>125</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>126</v>
       </c>
@@ -2346,7 +2345,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>128</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>129</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>132</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>133</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>134</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>137</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>138</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>140</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>141</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>142</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>143</v>
       </c>
@@ -2505,7 +2504,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>144</v>
       </c>
@@ -2519,7 +2518,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>146</v>
       </c>
@@ -2533,7 +2532,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>147</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>148</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>149</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>151</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>152</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>153</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>154</v>
       </c>
@@ -2637,7 +2636,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>225</v>
       </c>
@@ -2645,10 +2644,10 @@
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>50</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>155</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>156</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>157</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>158</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>159</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>160</v>
       </c>
@@ -2725,7 +2724,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>161</v>
       </c>
@@ -2743,103 +2742,103 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="G182" sqref="G182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.265625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.265625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" style="1" customWidth="1"/>
     <col min="29" max="29" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="22.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="9.1328125" style="1"/>
+    <col min="85" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>196</v>
       </c>
@@ -2856,7 +2855,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2887,7 +2886,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -2949,7 +2948,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -2994,7 +2993,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -3008,7 +3007,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>48</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>50</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
@@ -3138,7 +3137,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>61</v>
       </c>
@@ -3155,7 +3154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>61</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
@@ -3206,7 +3205,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -3240,7 +3239,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
@@ -3257,7 +3256,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
@@ -3274,7 +3273,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3308,7 +3307,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -3325,7 +3324,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -3342,7 +3341,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -3376,7 +3375,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -3393,7 +3392,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -3410,7 +3409,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
@@ -3427,7 +3426,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -3478,7 +3477,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -3506,7 +3505,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -3538,7 +3537,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>77</v>
       </c>
@@ -3555,7 +3554,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>77</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>77</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>77</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>77</v>
       </c>
@@ -3623,7 +3622,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>77</v>
       </c>
@@ -3640,7 +3639,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>77</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
@@ -3674,7 +3673,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>77</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
@@ -3708,7 +3707,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>77</v>
       </c>
@@ -3725,7 +3724,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>77</v>
       </c>
@@ -3742,7 +3741,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>77</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>78</v>
       </c>
@@ -3774,7 +3773,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>78</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>78</v>
       </c>
@@ -3825,7 +3824,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>78</v>
       </c>
@@ -3842,7 +3841,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>78</v>
       </c>
@@ -3859,7 +3858,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>78</v>
       </c>
@@ -3876,7 +3875,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>78</v>
       </c>
@@ -3893,7 +3892,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>78</v>
       </c>
@@ -3910,7 +3909,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>78</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
@@ -3944,7 +3943,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>78</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>78</v>
       </c>
@@ -3978,7 +3977,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>78</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>78</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>79</v>
       </c>
@@ -4027,7 +4026,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>79</v>
       </c>
@@ -4044,7 +4043,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>79</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>79</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>79</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>79</v>
       </c>
@@ -4112,7 +4111,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>79</v>
       </c>
@@ -4129,7 +4128,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>79</v>
       </c>
@@ -4146,7 +4145,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
@@ -4163,7 +4162,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>79</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>79</v>
       </c>
@@ -4197,7 +4196,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>79</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>79</v>
       </c>
@@ -4248,7 +4247,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>79</v>
       </c>
@@ -4265,7 +4264,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>80</v>
       </c>
@@ -4279,7 +4278,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>80</v>
       </c>
@@ -4296,7 +4295,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>80</v>
       </c>
@@ -4313,7 +4312,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>80</v>
       </c>
@@ -4330,7 +4329,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>80</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>80</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>80</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>80</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>80</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>80</v>
       </c>
@@ -4432,7 +4431,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>80</v>
       </c>
@@ -4449,7 +4448,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>80</v>
       </c>
@@ -4466,7 +4465,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>80</v>
       </c>
@@ -4483,7 +4482,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>80</v>
       </c>
@@ -4500,7 +4499,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>80</v>
       </c>
@@ -4517,7 +4516,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>81</v>
       </c>
@@ -4531,7 +4530,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>81</v>
       </c>
@@ -4548,7 +4547,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>81</v>
       </c>
@@ -4565,7 +4564,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>81</v>
       </c>
@@ -4582,7 +4581,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>81</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>81</v>
       </c>
@@ -4616,7 +4615,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>81</v>
       </c>
@@ -4633,7 +4632,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>81</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>81</v>
       </c>
@@ -4667,7 +4666,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>81</v>
       </c>
@@ -4684,7 +4683,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>81</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>81</v>
       </c>
@@ -4718,7 +4717,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>81</v>
       </c>
@@ -4735,7 +4734,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>81</v>
       </c>
@@ -4752,7 +4751,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>81</v>
       </c>
@@ -4769,7 +4768,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>85</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>85</v>
       </c>
@@ -4797,7 +4796,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>85</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>85</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>86</v>
       </c>
@@ -4839,7 +4838,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>86</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>86</v>
       </c>
@@ -4867,7 +4866,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>86</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>88</v>
       </c>
@@ -4895,7 +4894,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>89</v>
       </c>
@@ -4909,7 +4908,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>96</v>
       </c>
@@ -4923,7 +4922,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>97</v>
       </c>
@@ -4937,7 +4936,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>100</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>106</v>
       </c>
@@ -4965,7 +4964,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>128</v>
       </c>
@@ -4982,7 +4981,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>128</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>128</v>
       </c>
@@ -5016,7 +5015,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>128</v>
       </c>
@@ -5033,7 +5032,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>128</v>
       </c>
@@ -5050,7 +5049,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>128</v>
       </c>
@@ -5067,7 +5066,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>128</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>128</v>
       </c>
@@ -5101,7 +5100,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>128</v>
       </c>
@@ -5118,7 +5117,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>128</v>
       </c>
@@ -5135,7 +5134,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>128</v>
       </c>
@@ -5152,7 +5151,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>128</v>
       </c>
@@ -5169,7 +5168,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>128</v>
       </c>
@@ -5186,7 +5185,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>128</v>
       </c>
@@ -5203,7 +5202,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>128</v>
       </c>
@@ -5220,7 +5219,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>128</v>
       </c>
@@ -5237,7 +5236,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>128</v>
       </c>
@@ -5254,7 +5253,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>128</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>128</v>
       </c>
@@ -5288,7 +5287,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>129</v>
       </c>
@@ -5305,7 +5304,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>129</v>
       </c>
@@ -5322,7 +5321,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>129</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>129</v>
       </c>
@@ -5356,7 +5355,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>129</v>
       </c>
@@ -5373,7 +5372,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>129</v>
       </c>
@@ -5390,7 +5389,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>129</v>
       </c>
@@ -5407,7 +5406,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>129</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>129</v>
       </c>
@@ -5441,7 +5440,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>129</v>
       </c>
@@ -5458,7 +5457,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>129</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>129</v>
       </c>
@@ -5492,7 +5491,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>129</v>
       </c>
@@ -5509,7 +5508,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="163" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>129</v>
       </c>
@@ -5526,7 +5525,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>129</v>
       </c>
@@ -5543,7 +5542,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>129</v>
       </c>
@@ -5560,7 +5559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>129</v>
       </c>
@@ -5577,7 +5576,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>129</v>
       </c>
@@ -5594,7 +5593,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>129</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>137</v>
       </c>
@@ -5625,7 +5624,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>138</v>
       </c>
@@ -5639,7 +5638,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>144</v>
       </c>
@@ -5653,7 +5652,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>146</v>
       </c>
@@ -5667,7 +5666,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>147</v>
       </c>
@@ -5681,7 +5680,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>147</v>
       </c>
@@ -5698,7 +5697,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>147</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>147</v>
       </c>
@@ -5732,7 +5731,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>147</v>
       </c>
@@ -5749,7 +5748,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>147</v>
       </c>
@@ -5766,7 +5765,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>147</v>
       </c>
@@ -5783,7 +5782,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>147</v>
       </c>
@@ -5800,7 +5799,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>147</v>
       </c>
@@ -5817,7 +5816,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>147</v>
       </c>
@@ -5834,7 +5833,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>147</v>
       </c>
@@ -5851,7 +5850,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>147</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>148</v>
       </c>
@@ -5882,7 +5881,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>148</v>
       </c>
@@ -5899,7 +5898,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>148</v>
       </c>
@@ -5916,7 +5915,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>148</v>
       </c>
@@ -5933,7 +5932,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>148</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>148</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>148</v>
       </c>
@@ -5984,7 +5983,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>148</v>
       </c>
@@ -6001,7 +6000,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>148</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>148</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>148</v>
       </c>
@@ -6052,7 +6051,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>148</v>
       </c>
@@ -6069,7 +6068,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>149</v>
       </c>
@@ -6083,7 +6082,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>149</v>
       </c>
@@ -6100,7 +6099,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>149</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>149</v>
       </c>
@@ -6134,7 +6133,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>149</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>149</v>
       </c>
@@ -6168,7 +6167,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>149</v>
       </c>
@@ -6185,7 +6184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>149</v>
       </c>
@@ -6202,7 +6201,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>149</v>
       </c>
@@ -6219,7 +6218,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>149</v>
       </c>
@@ -6236,7 +6235,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>149</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>149</v>
       </c>
@@ -6271,9 +6270,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E208" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:E208"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6283,99 +6282,99 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>150</v>
       </c>
@@ -6386,30 +6385,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H149"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E19" sqref="A19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.73046875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="20" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="14"/>
+    <col min="3" max="3" width="9.140625" style="14"/>
     <col min="4" max="4" width="14" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.73046875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.265625" style="3" customWidth="1"/>
-    <col min="10" max="13" width="11.265625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.1328125" style="3"/>
-    <col min="15" max="15" width="18.3984375" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.1328125" style="3"/>
+    <col min="5" max="5" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
+    <col min="10" max="13" width="11.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="18.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>163</v>
       </c>
@@ -6428,7 +6427,7 @@
       <c r="G1"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>166</v>
       </c>
@@ -6444,7 +6443,7 @@
       <c r="G2"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>166</v>
       </c>
@@ -6460,7 +6459,7 @@
       <c r="G3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>166</v>
       </c>
@@ -6476,7 +6475,7 @@
       <c r="G4"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>166</v>
       </c>
@@ -6492,7 +6491,7 @@
       <c r="G5"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>166</v>
       </c>
@@ -6508,7 +6507,7 @@
       <c r="G6"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>166</v>
       </c>
@@ -6524,7 +6523,7 @@
       <c r="G7"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>166</v>
       </c>
@@ -6540,7 +6539,7 @@
       <c r="G8"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>168</v>
       </c>
@@ -6556,7 +6555,7 @@
       <c r="G9"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>168</v>
       </c>
@@ -6572,7 +6571,7 @@
       <c r="G10"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>168</v>
       </c>
@@ -6588,7 +6587,7 @@
       <c r="G11"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>168</v>
       </c>
@@ -6604,7 +6603,7 @@
       <c r="G12"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>168</v>
       </c>
@@ -6620,7 +6619,7 @@
       <c r="G13"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>168</v>
       </c>
@@ -6636,7 +6635,7 @@
       <c r="G14"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>168</v>
       </c>
@@ -6652,7 +6651,7 @@
       <c r="G15"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>168</v>
       </c>
@@ -6668,7 +6667,7 @@
       <c r="G16"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>168</v>
       </c>
@@ -6684,7 +6683,7 @@
       <c r="G17"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>168</v>
       </c>
@@ -6700,7 +6699,7 @@
       <c r="G18"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>168</v>
       </c>
@@ -6716,7 +6715,7 @@
       <c r="G19"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>168</v>
       </c>
@@ -6732,7 +6731,7 @@
       <c r="G20"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>168</v>
       </c>
@@ -6748,7 +6747,7 @@
       <c r="G21"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>168</v>
       </c>
@@ -6764,7 +6763,7 @@
       <c r="G22"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>168</v>
       </c>
@@ -6780,7 +6779,7 @@
       <c r="G23"/>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>168</v>
       </c>
@@ -6796,7 +6795,7 @@
       <c r="G24"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>175</v>
       </c>
@@ -6812,7 +6811,7 @@
       <c r="G25"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>175</v>
       </c>
@@ -6828,7 +6827,7 @@
       <c r="G26"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>175</v>
       </c>
@@ -6844,7 +6843,7 @@
       <c r="G27"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>175</v>
       </c>
@@ -6860,7 +6859,7 @@
       <c r="G28"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>175</v>
       </c>
@@ -6876,7 +6875,7 @@
       <c r="G29"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>175</v>
       </c>
@@ -6892,7 +6891,7 @@
       <c r="G30"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>175</v>
       </c>
@@ -6908,7 +6907,7 @@
       <c r="G31"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>175</v>
       </c>
@@ -6924,7 +6923,7 @@
       <c r="G32"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>179</v>
       </c>
@@ -6943,7 +6942,7 @@
       <c r="G33"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>179</v>
       </c>
@@ -6962,7 +6961,7 @@
       <c r="G34"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>179</v>
       </c>
@@ -6981,7 +6980,7 @@
       <c r="G35"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>179</v>
       </c>
@@ -7000,7 +6999,7 @@
       <c r="G36"/>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>179</v>
       </c>
@@ -7019,7 +7018,7 @@
       <c r="G37"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>179</v>
       </c>
@@ -7038,7 +7037,7 @@
       <c r="G38"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>179</v>
       </c>
@@ -7057,7 +7056,7 @@
       <c r="G39"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>179</v>
       </c>
@@ -7076,7 +7075,7 @@
       <c r="G40"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>179</v>
       </c>
@@ -7095,7 +7094,7 @@
       <c r="G41"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>179</v>
       </c>
@@ -7114,7 +7113,7 @@
       <c r="G42"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>179</v>
       </c>
@@ -7133,7 +7132,7 @@
       <c r="G43"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>179</v>
       </c>
@@ -7152,7 +7151,7 @@
       <c r="G44"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>179</v>
       </c>
@@ -7171,7 +7170,7 @@
       <c r="G45"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>179</v>
       </c>
@@ -7190,7 +7189,7 @@
       <c r="G46"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>179</v>
       </c>
@@ -7209,7 +7208,7 @@
       <c r="G47"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>179</v>
       </c>
@@ -7228,7 +7227,7 @@
       <c r="G48"/>
       <c r="H48" s="3"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>179</v>
       </c>
@@ -7247,7 +7246,7 @@
       <c r="G49"/>
       <c r="H49" s="3"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>179</v>
       </c>
@@ -7266,7 +7265,7 @@
       <c r="G50"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>179</v>
       </c>
@@ -7285,7 +7284,7 @@
       <c r="G51"/>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>179</v>
       </c>
@@ -7304,7 +7303,7 @@
       <c r="G52"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>179</v>
       </c>
@@ -7323,7 +7322,7 @@
       <c r="G53"/>
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>179</v>
       </c>
@@ -7342,7 +7341,7 @@
       <c r="G54"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>179</v>
       </c>
@@ -7361,7 +7360,7 @@
       <c r="G55"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>179</v>
       </c>
@@ -7380,7 +7379,7 @@
       <c r="G56"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>179</v>
       </c>
@@ -7399,7 +7398,7 @@
       <c r="G57"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>179</v>
       </c>
@@ -7418,7 +7417,7 @@
       <c r="G58"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>179</v>
       </c>
@@ -7437,7 +7436,7 @@
       <c r="G59"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>179</v>
       </c>
@@ -7456,7 +7455,7 @@
       <c r="G60"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>179</v>
       </c>
@@ -7475,7 +7474,7 @@
       <c r="G61"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>179</v>
       </c>
@@ -7494,7 +7493,7 @@
       <c r="G62"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>179</v>
       </c>
@@ -7513,7 +7512,7 @@
       <c r="G63"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>179</v>
       </c>
@@ -7532,7 +7531,7 @@
       <c r="G64"/>
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>179</v>
       </c>
@@ -7551,7 +7550,7 @@
       <c r="G65"/>
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>179</v>
       </c>
@@ -7570,7 +7569,7 @@
       <c r="G66"/>
       <c r="H66" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>179</v>
       </c>
@@ -7589,7 +7588,7 @@
       <c r="G67"/>
       <c r="H67" s="3"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>179</v>
       </c>
@@ -7608,7 +7607,7 @@
       <c r="G68"/>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>179</v>
       </c>
@@ -7627,7 +7626,7 @@
       <c r="G69"/>
       <c r="H69" s="3"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>179</v>
       </c>
@@ -7646,7 +7645,7 @@
       <c r="G70"/>
       <c r="H70" s="3"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>179</v>
       </c>
@@ -7665,7 +7664,7 @@
       <c r="G71"/>
       <c r="H71" s="3"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>179</v>
       </c>
@@ -7684,7 +7683,7 @@
       <c r="G72"/>
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>179</v>
       </c>
@@ -7703,7 +7702,7 @@
       <c r="G73"/>
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>179</v>
       </c>
@@ -7722,7 +7721,7 @@
       <c r="G74"/>
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>179</v>
       </c>
@@ -7741,7 +7740,7 @@
       <c r="G75"/>
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>179</v>
       </c>
@@ -7760,7 +7759,7 @@
       <c r="G76"/>
       <c r="H76" s="3"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>179</v>
       </c>
@@ -7779,7 +7778,7 @@
       <c r="G77"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>179</v>
       </c>
@@ -7798,7 +7797,7 @@
       <c r="G78"/>
       <c r="H78" s="3"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>179</v>
       </c>
@@ -7817,7 +7816,7 @@
       <c r="G79"/>
       <c r="H79" s="3"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>179</v>
       </c>
@@ -7836,7 +7835,7 @@
       <c r="G80"/>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>179</v>
       </c>
@@ -7855,7 +7854,7 @@
       <c r="G81"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>179</v>
       </c>
@@ -7874,7 +7873,7 @@
       <c r="G82"/>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>179</v>
       </c>
@@ -7893,7 +7892,7 @@
       <c r="G83"/>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>179</v>
       </c>
@@ -7912,7 +7911,7 @@
       <c r="G84"/>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>179</v>
       </c>
@@ -7931,7 +7930,7 @@
       <c r="G85"/>
       <c r="H85" s="3"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>179</v>
       </c>
@@ -7949,7 +7948,7 @@
       </c>
       <c r="H86" s="3"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>179</v>
       </c>
@@ -7967,7 +7966,7 @@
       </c>
       <c r="H87" s="3"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>179</v>
       </c>
@@ -7985,7 +7984,7 @@
       </c>
       <c r="H88" s="3"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>179</v>
       </c>
@@ -8003,7 +8002,7 @@
       </c>
       <c r="H89" s="3"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>179</v>
       </c>
@@ -8021,7 +8020,7 @@
       </c>
       <c r="H90" s="3"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>179</v>
       </c>
@@ -8039,7 +8038,7 @@
       </c>
       <c r="H91" s="3"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>179</v>
       </c>
@@ -8057,7 +8056,7 @@
       </c>
       <c r="H92" s="3"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>179</v>
       </c>
@@ -8075,7 +8074,7 @@
       </c>
       <c r="H93" s="3"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>179</v>
       </c>
@@ -8093,7 +8092,7 @@
       </c>
       <c r="H94" s="3"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>179</v>
       </c>
@@ -8111,7 +8110,7 @@
       </c>
       <c r="H95" s="3"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>179</v>
       </c>
@@ -8129,7 +8128,7 @@
       </c>
       <c r="H96" s="3"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>179</v>
       </c>
@@ -8147,7 +8146,7 @@
       </c>
       <c r="H97" s="3"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>179</v>
       </c>
@@ -8165,7 +8164,7 @@
       </c>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>179</v>
       </c>
@@ -8183,7 +8182,7 @@
       </c>
       <c r="H99" s="3"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>179</v>
       </c>
@@ -8201,7 +8200,7 @@
       </c>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>179</v>
       </c>
@@ -8219,7 +8218,7 @@
       </c>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>179</v>
       </c>
@@ -8237,7 +8236,7 @@
       </c>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>179</v>
       </c>
@@ -8255,7 +8254,7 @@
       </c>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>179</v>
       </c>
@@ -8273,7 +8272,7 @@
       </c>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>179</v>
       </c>
@@ -8291,7 +8290,7 @@
       </c>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>179</v>
       </c>
@@ -8309,7 +8308,7 @@
       </c>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>179</v>
       </c>
@@ -8327,7 +8326,7 @@
       </c>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
         <v>179</v>
       </c>
@@ -8345,7 +8344,7 @@
       </c>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>179</v>
       </c>
@@ -8363,7 +8362,7 @@
       </c>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>179</v>
       </c>
@@ -8381,7 +8380,7 @@
       </c>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
         <v>179</v>
       </c>
@@ -8399,7 +8398,7 @@
       </c>
       <c r="H111" s="3"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>179</v>
       </c>
@@ -8417,7 +8416,7 @@
       </c>
       <c r="H112" s="3"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>179</v>
       </c>
@@ -8435,7 +8434,7 @@
       </c>
       <c r="H113" s="3"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>179</v>
       </c>
@@ -8453,7 +8452,7 @@
       </c>
       <c r="H114" s="3"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>179</v>
       </c>
@@ -8471,7 +8470,7 @@
       </c>
       <c r="H115" s="3"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>179</v>
       </c>
@@ -8489,7 +8488,7 @@
       </c>
       <c r="H116" s="3"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>179</v>
       </c>
@@ -8507,7 +8506,7 @@
       </c>
       <c r="H117" s="3"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>179</v>
       </c>
@@ -8525,7 +8524,7 @@
       </c>
       <c r="H118" s="3"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>179</v>
       </c>
@@ -8543,7 +8542,7 @@
       </c>
       <c r="H119" s="3"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>179</v>
       </c>
@@ -8561,7 +8560,7 @@
       </c>
       <c r="H120" s="3"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>179</v>
       </c>
@@ -8579,7 +8578,7 @@
       </c>
       <c r="H121" s="3"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
         <v>179</v>
       </c>
@@ -8597,7 +8596,7 @@
       </c>
       <c r="H122" s="3"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
         <v>179</v>
       </c>
@@ -8615,7 +8614,7 @@
       </c>
       <c r="H123" s="3"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
         <v>179</v>
       </c>
@@ -8634,7 +8633,7 @@
       <c r="G124"/>
       <c r="H124" s="3"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
         <v>179</v>
       </c>
@@ -8653,7 +8652,7 @@
       <c r="G125"/>
       <c r="H125" s="3"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="9" t="s">
         <v>179</v>
       </c>
@@ -8672,7 +8671,7 @@
       <c r="G126"/>
       <c r="H126" s="3"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
         <v>179</v>
       </c>
@@ -8691,7 +8690,7 @@
       <c r="G127"/>
       <c r="H127" s="3"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
         <v>179</v>
       </c>
@@ -8710,7 +8709,7 @@
       <c r="G128"/>
       <c r="H128" s="3"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>179</v>
       </c>
@@ -8729,7 +8728,7 @@
       <c r="G129"/>
       <c r="H129" s="3"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>179</v>
       </c>
@@ -8748,7 +8747,7 @@
       <c r="G130"/>
       <c r="H130" s="3"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>179</v>
       </c>
@@ -8767,7 +8766,7 @@
       <c r="G131"/>
       <c r="H131" s="3"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>179</v>
       </c>
@@ -8786,7 +8785,7 @@
       <c r="G132"/>
       <c r="H132" s="3"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>179</v>
       </c>
@@ -8805,7 +8804,7 @@
       <c r="G133"/>
       <c r="H133" s="3"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>179</v>
       </c>
@@ -8824,7 +8823,7 @@
       <c r="G134"/>
       <c r="H134" s="3"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>179</v>
       </c>
@@ -8843,7 +8842,7 @@
       <c r="G135"/>
       <c r="H135" s="3"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>179</v>
       </c>
@@ -8862,7 +8861,7 @@
       <c r="G136"/>
       <c r="H136" s="3"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>179</v>
       </c>
@@ -8881,7 +8880,7 @@
       <c r="G137"/>
       <c r="H137" s="3"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>179</v>
       </c>
@@ -8900,7 +8899,7 @@
       <c r="G138"/>
       <c r="H138" s="3"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>179</v>
       </c>
@@ -8919,7 +8918,7 @@
       <c r="G139"/>
       <c r="H139" s="3"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>179</v>
       </c>
@@ -8938,7 +8937,7 @@
       <c r="G140"/>
       <c r="H140" s="3"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>179</v>
       </c>
@@ -8957,7 +8956,7 @@
       <c r="G141"/>
       <c r="H141" s="3"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>179</v>
       </c>
@@ -8976,7 +8975,7 @@
       <c r="G142"/>
       <c r="H142" s="3"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>179</v>
       </c>
@@ -8995,7 +8994,7 @@
       <c r="G143"/>
       <c r="H143" s="3"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
         <v>179</v>
       </c>
@@ -9014,7 +9013,7 @@
       <c r="G144"/>
       <c r="H144" s="3"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
         <v>179</v>
       </c>
@@ -9033,7 +9032,7 @@
       <c r="G145"/>
       <c r="H145" s="3"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
         <v>179</v>
       </c>
@@ -9052,7 +9051,7 @@
       <c r="G146"/>
       <c r="H146" s="3"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
         <v>179</v>
       </c>
@@ -9071,7 +9070,7 @@
       <c r="G147"/>
       <c r="H147" s="3"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>179</v>
       </c>
@@ -9090,7 +9089,7 @@
       <c r="G148"/>
       <c r="H148" s="3"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
         <v>179</v>
       </c>
@@ -9110,7 +9109,7 @@
       <c r="H149" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E149" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:E149"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add 25F_25A group and variants to template
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Serotype" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="4. Variants" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. SerotypeVariants'!$A$1:$E$208</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Variants'!$A$1:$E$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. SerotypeVariants'!$A$1:$E$220</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Variants'!$A$1:$E$161</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="232">
   <si>
     <t>serotype_1</t>
   </si>
@@ -722,6 +722,12 @@
   </si>
   <si>
     <t>func</t>
+  </si>
+  <si>
+    <t>25F_25A</t>
+  </si>
+  <si>
+    <t>wcyC</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,8 +2327,11 @@
       <c r="A63" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C63" s="3" t="b">
-        <v>0</v>
+      <c r="B63" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>125</v>
@@ -2335,8 +2344,11 @@
       <c r="A64" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="3" t="b">
-        <v>0</v>
+      <c r="B64" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>125</v>
@@ -2743,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4966,206 +4978,206 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D131" s="1">
-        <v>39</v>
+        <v>231</v>
+      </c>
+      <c r="D131" s="21">
+        <v>143</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D132" s="1">
-        <v>71</v>
+        <v>231</v>
+      </c>
+      <c r="D132" s="21">
+        <v>155</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D133" s="22">
-        <v>84</v>
+        <v>231</v>
+      </c>
+      <c r="D133" s="21">
+        <v>191</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D134" s="22">
-        <v>245</v>
+        <v>231</v>
+      </c>
+      <c r="D134" s="21">
+        <v>220</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D135" s="22">
-        <v>246</v>
+        <v>231</v>
+      </c>
+      <c r="D135" s="21">
+        <v>297</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D136" s="22">
-        <v>247</v>
+        <v>231</v>
+      </c>
+      <c r="D136" s="21">
+        <v>301</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D137" s="1">
-        <v>250</v>
+        <v>231</v>
+      </c>
+      <c r="D137" s="21">
+        <v>143</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D138" s="22">
-        <v>256</v>
+        <v>231</v>
+      </c>
+      <c r="D138" s="21">
+        <v>155</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D139" s="1">
-        <v>260</v>
+        <v>231</v>
+      </c>
+      <c r="D139" s="21">
+        <v>191</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D140" s="1">
-        <v>279</v>
+        <v>231</v>
+      </c>
+      <c r="D140" s="21">
+        <v>220</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D141" s="1">
-        <v>293</v>
+        <v>231</v>
+      </c>
+      <c r="D141" s="21">
+        <v>297</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D142" s="1">
-        <v>294</v>
+        <v>231</v>
+      </c>
+      <c r="D142" s="21">
+        <v>301</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -5179,10 +5191,10 @@
         <v>185</v>
       </c>
       <c r="D143" s="1">
-        <v>297</v>
+        <v>39</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -5196,10 +5208,10 @@
         <v>185</v>
       </c>
       <c r="D144" s="1">
-        <v>298</v>
+        <v>71</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -5212,11 +5224,11 @@
       <c r="C145" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D145" s="1">
-        <v>304</v>
+      <c r="D145" s="22">
+        <v>84</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -5229,11 +5241,11 @@
       <c r="C146" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D146" s="1">
-        <v>328</v>
+      <c r="D146" s="22">
+        <v>245</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -5246,11 +5258,11 @@
       <c r="C147" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D147" s="1">
-        <v>341</v>
+      <c r="D147" s="22">
+        <v>246</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -5263,11 +5275,11 @@
       <c r="C148" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D148" s="1">
-        <v>342</v>
+      <c r="D148" s="22">
+        <v>247</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5281,15 +5293,15 @@
         <v>185</v>
       </c>
       <c r="D149" s="1">
-        <v>345</v>
+        <v>250</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>179</v>
@@ -5297,16 +5309,16 @@
       <c r="C150" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D150" s="1">
-        <v>39</v>
+      <c r="D150" s="22">
+        <v>256</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>179</v>
@@ -5315,15 +5327,15 @@
         <v>185</v>
       </c>
       <c r="D151" s="1">
-        <v>71</v>
+        <v>260</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>179</v>
@@ -5331,16 +5343,16 @@
       <c r="C152" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D152" s="22">
-        <v>84</v>
+      <c r="D152" s="1">
+        <v>279</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>179</v>
@@ -5348,16 +5360,16 @@
       <c r="C153" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D153" s="22">
-        <v>245</v>
+      <c r="D153" s="1">
+        <v>293</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>179</v>
@@ -5365,16 +5377,16 @@
       <c r="C154" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D154" s="22">
-        <v>246</v>
+      <c r="D154" s="1">
+        <v>294</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>179</v>
@@ -5382,16 +5394,16 @@
       <c r="C155" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D155" s="22">
-        <v>247</v>
+      <c r="D155" s="1">
+        <v>297</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>179</v>
@@ -5400,15 +5412,15 @@
         <v>185</v>
       </c>
       <c r="D156" s="1">
-        <v>250</v>
+        <v>298</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>179</v>
@@ -5416,16 +5428,16 @@
       <c r="C157" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D157" s="22">
-        <v>256</v>
+      <c r="D157" s="1">
+        <v>304</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>179</v>
@@ -5434,15 +5446,15 @@
         <v>185</v>
       </c>
       <c r="D158" s="1">
-        <v>260</v>
+        <v>328</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>179</v>
@@ -5451,15 +5463,15 @@
         <v>185</v>
       </c>
       <c r="D159" s="1">
-        <v>279</v>
+        <v>341</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>179</v>
@@ -5468,15 +5480,15 @@
         <v>185</v>
       </c>
       <c r="D160" s="1">
-        <v>293</v>
+        <v>342</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>179</v>
@@ -5485,10 +5497,10 @@
         <v>185</v>
       </c>
       <c r="D161" s="1">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5502,10 +5514,10 @@
         <v>185</v>
       </c>
       <c r="D162" s="1">
-        <v>297</v>
+        <v>39</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5519,10 +5531,10 @@
         <v>185</v>
       </c>
       <c r="D163" s="1">
-        <v>298</v>
+        <v>71</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5535,14 +5547,14 @@
       <c r="C164" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D164" s="1">
-        <v>304</v>
+      <c r="D164" s="22">
+        <v>84</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>129</v>
       </c>
@@ -5552,14 +5564,14 @@
       <c r="C165" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D165" s="1">
-        <v>328</v>
+      <c r="D165" s="22">
+        <v>245</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>129</v>
       </c>
@@ -5569,14 +5581,14 @@
       <c r="C166" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D166" s="1">
-        <v>341</v>
+      <c r="D166" s="22">
+        <v>246</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>129</v>
       </c>
@@ -5586,14 +5598,14 @@
       <c r="C167" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D167" s="1">
-        <v>342</v>
+      <c r="D167" s="22">
+        <v>247</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>129</v>
       </c>
@@ -5604,272 +5616,275 @@
         <v>185</v>
       </c>
       <c r="D168" s="1">
-        <v>345</v>
+        <v>250</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>170</v>
+        <v>185</v>
+      </c>
+      <c r="D169" s="22">
+        <v>256</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>170</v>
+        <v>185</v>
+      </c>
+      <c r="D170" s="1">
+        <v>260</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
+      </c>
+      <c r="D171" s="1">
+        <v>279</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
+      </c>
+      <c r="D172" s="1">
+        <v>293</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
+      </c>
+      <c r="D173" s="1">
+        <v>294</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D174" s="1">
-        <v>66</v>
+        <v>297</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D175" s="1">
-        <v>96</v>
+        <v>298</v>
       </c>
       <c r="E175" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D176" s="1">
+        <v>304</v>
+      </c>
+      <c r="E176" s="1" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D176" s="22">
-        <v>152</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D177" s="22">
-        <v>180</v>
+        <v>185</v>
+      </c>
+      <c r="D177" s="1">
+        <v>328</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D178" s="22">
-        <v>188</v>
+        <v>185</v>
+      </c>
+      <c r="D178" s="1">
+        <v>341</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D179" s="22">
-        <v>198</v>
+        <v>185</v>
+      </c>
+      <c r="D179" s="1">
+        <v>342</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>179</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D180" s="22">
-        <v>151</v>
+        <v>185</v>
+      </c>
+      <c r="D180" s="1">
+        <v>345</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D181" s="22">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D182" s="22">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D183" s="22">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D184" s="22">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>168</v>
@@ -5878,12 +5893,12 @@
         <v>191</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>179</v>
@@ -5891,16 +5906,16 @@
       <c r="C186" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D186" s="21">
+      <c r="D186" s="1">
         <v>66</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>179</v>
@@ -5908,16 +5923,16 @@
       <c r="C187" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D187" s="21">
+      <c r="D187" s="1">
         <v>96</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>179</v>
@@ -5929,12 +5944,12 @@
         <v>152</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>179</v>
@@ -5946,12 +5961,12 @@
         <v>180</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>179</v>
@@ -5963,12 +5978,12 @@
         <v>188</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>179</v>
@@ -5980,12 +5995,12 @@
         <v>198</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>179</v>
@@ -6002,7 +6017,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>179</v>
@@ -6019,7 +6034,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>179</v>
@@ -6036,7 +6051,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>179</v>
@@ -6053,7 +6068,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>179</v>
@@ -6070,7 +6085,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>168</v>
@@ -6084,7 +6099,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>179</v>
@@ -6101,7 +6116,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>179</v>
@@ -6118,7 +6133,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>179</v>
@@ -6135,7 +6150,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>179</v>
@@ -6152,7 +6167,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>179</v>
@@ -6169,7 +6184,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>179</v>
@@ -6186,7 +6201,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>179</v>
@@ -6198,12 +6213,12 @@
         <v>151</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>179</v>
@@ -6215,12 +6230,12 @@
         <v>155</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>179</v>
@@ -6232,12 +6247,12 @@
         <v>175</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>179</v>
@@ -6249,12 +6264,12 @@
         <v>176</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>179</v>
@@ -6266,11 +6281,212 @@
         <v>189</v>
       </c>
       <c r="E208" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D210" s="21">
+        <v>66</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D211" s="21">
+        <v>96</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D212" s="22">
+        <v>152</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D213" s="22">
+        <v>180</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D214" s="22">
+        <v>188</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D215" s="22">
+        <v>198</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D216" s="22">
+        <v>151</v>
+      </c>
+      <c r="E216" s="1" t="s">
         <v>220</v>
       </c>
     </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D217" s="22">
+        <v>155</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D218" s="22">
+        <v>175</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D219" s="22">
+        <v>176</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D220" s="22">
+        <v>189</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E208"/>
+  <autoFilter ref="A1:E220"/>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>0</formula1>
@@ -6283,10 +6499,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6361,21 +6577,26 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -6386,10 +6607,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H149"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E19" sqref="A19:E20"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8007,16 +8228,16 @@
         <v>179</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C90" s="14">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H90" s="3"/>
     </row>
@@ -8025,16 +8246,16 @@
         <v>179</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C91" s="14">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H91" s="3"/>
     </row>
@@ -8043,16 +8264,16 @@
         <v>179</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C92" s="14">
-        <v>71</v>
+        <v>191</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H92" s="3"/>
     </row>
@@ -8061,16 +8282,16 @@
         <v>179</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C93" s="14">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H93" s="3"/>
     </row>
@@ -8079,16 +8300,16 @@
         <v>179</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C94" s="14">
-        <v>84</v>
+        <v>297</v>
       </c>
       <c r="D94" s="18" t="s">
         <v>214</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H94" s="3"/>
     </row>
@@ -8097,16 +8318,16 @@
         <v>179</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C95" s="14">
-        <v>84</v>
+        <v>301</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H95" s="3"/>
     </row>
@@ -8115,16 +8336,16 @@
         <v>179</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C96" s="14">
-        <v>245</v>
+        <v>143</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H96" s="3"/>
     </row>
@@ -8133,16 +8354,16 @@
         <v>179</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C97" s="14">
-        <v>245</v>
+        <v>155</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H97" s="3"/>
     </row>
@@ -8150,17 +8371,17 @@
       <c r="A98" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B98" s="12" t="s">
-        <v>185</v>
+      <c r="B98" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="C98" s="14">
-        <v>246</v>
+        <v>191</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H98" s="3"/>
     </row>
@@ -8168,17 +8389,17 @@
       <c r="A99" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B99" s="12" t="s">
-        <v>185</v>
+      <c r="B99" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="C99" s="14">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H99" s="3"/>
     </row>
@@ -8187,16 +8408,16 @@
         <v>179</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C100" s="14">
-        <v>247</v>
+        <v>297</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H100" s="3"/>
     </row>
@@ -8205,16 +8426,16 @@
         <v>179</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>185</v>
+        <v>231</v>
       </c>
       <c r="C101" s="14">
-        <v>247</v>
+        <v>301</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="H101" s="3"/>
     </row>
@@ -8226,10 +8447,10 @@
         <v>185</v>
       </c>
       <c r="C102" s="14">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>130</v>
@@ -8244,10 +8465,10 @@
         <v>185</v>
       </c>
       <c r="C103" s="14">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>130</v>
@@ -8262,10 +8483,10 @@
         <v>185</v>
       </c>
       <c r="C104" s="14">
-        <v>256</v>
+        <v>71</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>130</v>
@@ -8280,10 +8501,10 @@
         <v>185</v>
       </c>
       <c r="C105" s="14">
-        <v>256</v>
+        <v>71</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>130</v>
@@ -8298,10 +8519,10 @@
         <v>185</v>
       </c>
       <c r="C106" s="14">
-        <v>260</v>
+        <v>84</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>130</v>
@@ -8316,10 +8537,10 @@
         <v>185</v>
       </c>
       <c r="C107" s="14">
-        <v>260</v>
+        <v>84</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>130</v>
@@ -8334,10 +8555,10 @@
         <v>185</v>
       </c>
       <c r="C108" s="14">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>130</v>
@@ -8352,10 +8573,10 @@
         <v>185</v>
       </c>
       <c r="C109" s="14">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>130</v>
@@ -8366,14 +8587,14 @@
       <c r="A110" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B110" s="12" t="s">
         <v>185</v>
       </c>
       <c r="C110" s="14">
-        <v>293</v>
+        <v>246</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>130</v>
@@ -8384,14 +8605,14 @@
       <c r="A111" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="12" t="s">
         <v>185</v>
       </c>
       <c r="C111" s="14">
-        <v>293</v>
+        <v>246</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>130</v>
@@ -8406,10 +8627,10 @@
         <v>185</v>
       </c>
       <c r="C112" s="14">
-        <v>294</v>
+        <v>247</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>130</v>
@@ -8424,10 +8645,10 @@
         <v>185</v>
       </c>
       <c r="C113" s="14">
-        <v>294</v>
+        <v>247</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>130</v>
@@ -8442,10 +8663,10 @@
         <v>185</v>
       </c>
       <c r="C114" s="14">
-        <v>297</v>
+        <v>250</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>130</v>
@@ -8460,10 +8681,10 @@
         <v>185</v>
       </c>
       <c r="C115" s="14">
-        <v>297</v>
+        <v>250</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E115" s="7" t="s">
         <v>130</v>
@@ -8478,10 +8699,10 @@
         <v>185</v>
       </c>
       <c r="C116" s="14">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>130</v>
@@ -8496,10 +8717,10 @@
         <v>185</v>
       </c>
       <c r="C117" s="14">
-        <v>298</v>
+        <v>256</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>130</v>
@@ -8514,10 +8735,10 @@
         <v>185</v>
       </c>
       <c r="C118" s="14">
-        <v>304</v>
+        <v>260</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>130</v>
@@ -8532,10 +8753,10 @@
         <v>185</v>
       </c>
       <c r="C119" s="14">
-        <v>304</v>
+        <v>260</v>
       </c>
       <c r="D119" s="18" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>130</v>
@@ -8550,10 +8771,10 @@
         <v>185</v>
       </c>
       <c r="C120" s="14">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>130</v>
@@ -8568,10 +8789,10 @@
         <v>185</v>
       </c>
       <c r="C121" s="14">
-        <v>328</v>
+        <v>279</v>
       </c>
       <c r="D121" s="18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E121" s="7" t="s">
         <v>130</v>
@@ -8586,7 +8807,7 @@
         <v>185</v>
       </c>
       <c r="C122" s="14">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="D122" s="18" t="s">
         <v>213</v>
@@ -8604,10 +8825,10 @@
         <v>185</v>
       </c>
       <c r="C123" s="14">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>130</v>
@@ -8622,15 +8843,14 @@
         <v>185</v>
       </c>
       <c r="C124" s="14">
-        <v>342</v>
+        <v>294</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G124"/>
       <c r="H124" s="3"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -8641,15 +8861,14 @@
         <v>185</v>
       </c>
       <c r="C125" s="14">
-        <v>342</v>
+        <v>294</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G125"/>
       <c r="H125" s="3"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -8660,15 +8879,14 @@
         <v>185</v>
       </c>
       <c r="C126" s="14">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G126"/>
       <c r="H126" s="3"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -8679,15 +8897,14 @@
         <v>185</v>
       </c>
       <c r="C127" s="14">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G127"/>
       <c r="H127" s="3"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -8695,18 +8912,17 @@
         <v>179</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C128" s="14">
-        <v>66</v>
+        <v>298</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>220</v>
       </c>
       <c r="E128" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G128"/>
+        <v>130</v>
+      </c>
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -8714,18 +8930,17 @@
         <v>179</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C129" s="14">
-        <v>66</v>
+        <v>298</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G129"/>
+        <v>130</v>
+      </c>
       <c r="H129" s="3"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -8733,18 +8948,17 @@
         <v>179</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C130" s="14">
-        <v>96</v>
+        <v>304</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G130"/>
+        <v>130</v>
+      </c>
       <c r="H130" s="3"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -8752,18 +8966,17 @@
         <v>179</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C131" s="14">
-        <v>96</v>
+        <v>304</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G131"/>
+        <v>130</v>
+      </c>
       <c r="H131" s="3"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -8771,18 +8984,17 @@
         <v>179</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C132" s="14">
-        <v>152</v>
+        <v>328</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G132"/>
+        <v>130</v>
+      </c>
       <c r="H132" s="3"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -8790,18 +9002,17 @@
         <v>179</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C133" s="14">
-        <v>152</v>
+        <v>328</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G133"/>
+        <v>130</v>
+      </c>
       <c r="H133" s="3"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -8809,18 +9020,17 @@
         <v>179</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C134" s="14">
-        <v>180</v>
+        <v>341</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G134"/>
+        <v>130</v>
+      </c>
       <c r="H134" s="3"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -8828,18 +9038,17 @@
         <v>179</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C135" s="14">
-        <v>180</v>
+        <v>341</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="G135"/>
+        <v>130</v>
+      </c>
       <c r="H135" s="3"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -8847,16 +9056,16 @@
         <v>179</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C136" s="14">
-        <v>188</v>
+        <v>342</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="G136"/>
       <c r="H136" s="3"/>
@@ -8866,16 +9075,16 @@
         <v>179</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C137" s="14">
-        <v>188</v>
+        <v>342</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="G137"/>
       <c r="H137" s="3"/>
@@ -8885,16 +9094,16 @@
         <v>179</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C138" s="14">
-        <v>198</v>
+        <v>345</v>
       </c>
       <c r="D138" s="18" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="G138"/>
       <c r="H138" s="3"/>
@@ -8904,16 +9113,16 @@
         <v>179</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C139" s="14">
-        <v>198</v>
+        <v>345</v>
       </c>
       <c r="D139" s="18" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="G139"/>
       <c r="H139" s="3"/>
@@ -8923,13 +9132,13 @@
         <v>179</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C140" s="14">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="D140" s="18" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>150</v>
@@ -8942,13 +9151,13 @@
         <v>179</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C141" s="14">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="D141" s="18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E141" s="7" t="s">
         <v>150</v>
@@ -8961,13 +9170,13 @@
         <v>179</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C142" s="14">
-        <v>155</v>
+        <v>96</v>
       </c>
       <c r="D142" s="18" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E142" s="7" t="s">
         <v>150</v>
@@ -8980,13 +9189,13 @@
         <v>179</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C143" s="14">
-        <v>155</v>
+        <v>96</v>
       </c>
       <c r="D143" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E143" s="7" t="s">
         <v>150</v>
@@ -8999,13 +9208,13 @@
         <v>179</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C144" s="14">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D144" s="18" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>150</v>
@@ -9018,13 +9227,13 @@
         <v>179</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C145" s="14">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D145" s="18" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>150</v>
@@ -9037,13 +9246,13 @@
         <v>179</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C146" s="14">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D146" s="18" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>150</v>
@@ -9056,13 +9265,13 @@
         <v>179</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C147" s="14">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>150</v>
@@ -9075,13 +9284,13 @@
         <v>179</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C148" s="14">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D148" s="18" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>150</v>
@@ -9094,13 +9303,13 @@
         <v>179</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C149" s="14">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D149" s="18" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>150</v>
@@ -9108,8 +9317,236 @@
       <c r="G149"/>
       <c r="H149" s="3"/>
     </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C150" s="14">
+        <v>198</v>
+      </c>
+      <c r="D150" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G150"/>
+      <c r="H150" s="3"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C151" s="14">
+        <v>198</v>
+      </c>
+      <c r="D151" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G151"/>
+      <c r="H151" s="3"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C152" s="14">
+        <v>151</v>
+      </c>
+      <c r="D152" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G152"/>
+      <c r="H152" s="3"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A153" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C153" s="14">
+        <v>151</v>
+      </c>
+      <c r="D153" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G153"/>
+      <c r="H153" s="3"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A154" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C154" s="14">
+        <v>155</v>
+      </c>
+      <c r="D154" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G154"/>
+      <c r="H154" s="3"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A155" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C155" s="14">
+        <v>155</v>
+      </c>
+      <c r="D155" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G155"/>
+      <c r="H155" s="3"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A156" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C156" s="14">
+        <v>175</v>
+      </c>
+      <c r="D156" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G156"/>
+      <c r="H156" s="3"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C157" s="14">
+        <v>175</v>
+      </c>
+      <c r="D157" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G157"/>
+      <c r="H157" s="3"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C158" s="14">
+        <v>176</v>
+      </c>
+      <c r="D158" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G158"/>
+      <c r="H158" s="3"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C159" s="14">
+        <v>176</v>
+      </c>
+      <c r="D159" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G159"/>
+      <c r="H159" s="3"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C160" s="14">
+        <v>189</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E160" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G160"/>
+      <c r="H160" s="3"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C161" s="14">
+        <v>189</v>
+      </c>
+      <c r="D161" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G161"/>
+      <c r="H161" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E149"/>
+  <autoFilter ref="A1:E161"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix issue with ctvdb setup Fix issues with wcyD and wcyV mash sketches causing failed stage 2 for group 25/38
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -820,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M66" activeCellId="0" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2278,6 +2278,9 @@
       <c r="E81" s="2" t="s">
         <v>133</v>
       </c>
+      <c r="F81" s="2" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
@@ -2288,11 +2291,9 @@
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>162</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="F82" s="0"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">

</xml_diff>

<commit_message>
Added 24F2 and 33F2 references to initial reference in CTVdb to better represent circulating strains and improve hit scores for these serotypes. Needs validation on multiple isolates
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="195">
   <si>
     <t xml:space="preserve">predicted_pheno</t>
   </si>
@@ -457,6 +457,9 @@
     <t xml:space="preserve">24B</t>
   </si>
   <si>
+    <t xml:space="preserve">24F2</t>
+  </si>
+  <si>
     <t xml:space="preserve">24A</t>
   </si>
   <si>
@@ -509,6 +512,9 @@
   </si>
   <si>
     <t xml:space="preserve">33A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33F2</t>
   </si>
   <si>
     <t xml:space="preserve">33B</t>
@@ -820,8 +826,8 @@
   </sheetPr>
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M66" activeCellId="0" sqref="M66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1931,367 +1937,375 @@
       <c r="E58" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="F58" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C59" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C60" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C61" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="E62" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="E63" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C64" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C65" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C66" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C67" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E67" s="2" t="s">
-        <v>147</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C68" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="E68" s="2" t="s">
-        <v>147</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C69" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C70" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C71" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C72" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C73" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C74" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C74" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C75" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C76" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F76" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="C77" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F77" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C78" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C79" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C80" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C81" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="F81" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C82" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F82" s="0"/>
     </row>
@@ -2309,86 +2323,86 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C84" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C85" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C86" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C87" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C88" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C89" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C90" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2404,13 +2418,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2507,16 +2521,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,13 +2538,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,13 +2552,13 @@
         <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,13 +2566,13 @@
         <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,10 +2580,10 @@
         <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -2580,10 +2594,10 @@
         <v>88</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>18</v>
@@ -2594,13 +2608,13 @@
         <v>91</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,13 +2622,13 @@
         <v>91</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2622,13 +2636,13 @@
         <v>91</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2636,13 +2650,13 @@
         <v>91</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,13 +2664,13 @@
         <v>93</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,13 +2678,13 @@
         <v>93</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,13 +2692,13 @@
         <v>93</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2692,13 +2706,13 @@
         <v>93</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,10 +2720,10 @@
         <v>106</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>18</v>
@@ -2720,10 +2734,10 @@
         <v>112</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>20</v>
@@ -2731,61 +2745,60 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>185</v>
+      </c>
+    </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2796,14 +2809,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E21">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="allele"/>
-        <filter val="gene_presence"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E21"/>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1:D20" type="whole">
       <formula1>0</formula1>
@@ -2841,7 +2847,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,27 +2912,27 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2969,30 +2975,30 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>29</v>
@@ -3001,13 +3007,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>29</v>
@@ -3016,13 +3022,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>29</v>
@@ -3031,10 +3037,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
@@ -3046,10 +3052,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -3061,10 +3067,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -3076,10 +3082,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>20</v>
@@ -3091,43 +3097,43 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>92</v>
@@ -3136,13 +3142,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>92</v>
@@ -3151,13 +3157,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>92</v>
@@ -3166,13 +3172,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>92</v>
@@ -3181,13 +3187,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>92</v>
@@ -3196,13 +3202,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>92</v>
@@ -3211,13 +3217,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>92</v>
@@ -3226,13 +3232,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>92</v>
@@ -3241,32 +3247,32 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F19" s="4"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H20" s="3"/>
     </row>

</xml_diff>

<commit_message>
update version number, update import template
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="195">
   <si>
     <t xml:space="preserve">predicted_pheno</t>
   </si>
@@ -824,10 +824,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H75" activeCellId="0" sqref="H75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1124,65 +1124,27 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>49</v>
@@ -1200,25 +1162,25 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>54</v>
@@ -1236,49 +1198,49 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C16" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>62</v>
@@ -1296,25 +1258,25 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C18" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>67</v>
@@ -1332,85 +1294,85 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C20" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C22" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C24" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C25" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>77</v>
@@ -1428,25 +1390,25 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C27" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>80</v>
@@ -1464,25 +1426,34 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>83</v>
@@ -1508,59 +1479,50 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>83</v>
+      <c r="A31" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="C31" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C33" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>92</v>
@@ -1578,25 +1540,25 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C35" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>95</v>
@@ -1614,85 +1576,85 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C37" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C38" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C39" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C40" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C42" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>103</v>
@@ -1710,37 +1672,45 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C44" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>106</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>107</v>
@@ -1766,232 +1736,224 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>30</v>
+        <v>117</v>
+      </c>
+      <c r="C48" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C50" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C51" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C52" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C54" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C55" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>124</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>30</v>
+        <v>126</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C57" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C58" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="C59" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C60" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C61" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>137</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>139</v>
+      <c r="C62" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>137</v>
@@ -2002,64 +1964,68 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C63" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C64" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C65" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="C66" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>145</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>147</v>
@@ -2081,77 +2047,70 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C68" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G68" s="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C69" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C70" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C71" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C72" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>155</v>
@@ -2166,22 +2125,25 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C74" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>158</v>
@@ -2196,10 +2158,13 @@
       <c r="E75" s="2" t="s">
         <v>157</v>
       </c>
+      <c r="F75" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>158</v>
@@ -2220,191 +2185,171 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C77" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C78" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C79" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="C80" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>163</v>
+        <v>135</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="C81" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>164</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>165</v>
+        <v>56</v>
       </c>
       <c r="C82" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F82" s="0"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="C83" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C84" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C85" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C86" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C87" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C88" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C89" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C90" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updates to interpretations when median multiplicity is low
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -826,7 +826,7 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
@@ -2369,7 +2369,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2899,7 +2899,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix typo with 24F/24B group result
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -431,7 +431,7 @@
     <t xml:space="preserve">23F</t>
   </si>
   <si>
-    <t xml:space="preserve">24F/25B</t>
+    <t xml:space="preserve">24F/24B</t>
   </si>
   <si>
     <t xml:space="preserve">24F</t>
@@ -824,8 +824,8 @@
   </sheetPr>
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2057,7 +2057,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added sequences for non-capsular organisms.
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\PycharmProjects\PneumoKITy\Database_tools\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651B090A-9632-46E9-AEB4-B7B583DE2983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1. Serotype" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="2. SerotypeVariants" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="3. Group" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="4. Variants" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="1. Serotype" sheetId="1" r:id="rId1"/>
+    <sheet name="2. SerotypeVariants" sheetId="2" r:id="rId2"/>
+    <sheet name="3. Group" sheetId="3" r:id="rId3"/>
+    <sheet name="4. Variants" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'1. Serotype'!$A$1:$R$77</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2. SerotypeVariants'!$A$1:$E$21</definedName>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'4. Variants'!$A$1:$E$20</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'2. SerotypeVariants'!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Serotype'!$A$1:$R$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. SerotypeVariants'!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Variants'!$A$1:$E$20</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'2. SerotypeVariants'!$A$1:$E$20</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,21 +33,20 @@
 </workbook>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Carmen Sheppard:
@@ -53,7 +57,6 @@
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="0"/>
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">variant cannot = 0 
@@ -66,580 +69,589 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="187">
-  <si>
-    <t xml:space="preserve">predicted_pheno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stage2_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subtypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serotype_15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6A/6B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6A_6B_6C_6D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06A-VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06B-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06B-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06B-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06C-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6C/6D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serogroup_6_(6E)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7F/7A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7B/40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9A/9V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9N/9L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11A/11D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11B/11C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12F_12A_12B_44_46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12A/12B/44/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15F_15A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15B/15C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18C/18B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19A_19AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19A-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19A-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19A-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19F-I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19F-II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19F-III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19F-IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24F/24B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25F/25A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25F_25A_38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28F/28A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32F/32A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33F/33A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35B/35D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35A/35C/42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">var_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allele</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wciN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wciI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gene_presence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">detected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rmlB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rmlD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wcjE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not_detected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wzy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wcyD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wcyV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group_id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="191">
+  <si>
+    <t>predicted_pheno</t>
+  </si>
+  <si>
+    <t>stage2_group</t>
+  </si>
+  <si>
+    <t>subtypes</t>
+  </si>
+  <si>
+    <t>serotype_1</t>
+  </si>
+  <si>
+    <t>serotype_2</t>
+  </si>
+  <si>
+    <t>serotype_3</t>
+  </si>
+  <si>
+    <t>serotype_4</t>
+  </si>
+  <si>
+    <t>serotype_5</t>
+  </si>
+  <si>
+    <t>serotype_6</t>
+  </si>
+  <si>
+    <t>serotype_7</t>
+  </si>
+  <si>
+    <t>serotype_8</t>
+  </si>
+  <si>
+    <t>serotype_9</t>
+  </si>
+  <si>
+    <t>serotype_10</t>
+  </si>
+  <si>
+    <t>serotype_11</t>
+  </si>
+  <si>
+    <t>serotype_12</t>
+  </si>
+  <si>
+    <t>serotype_13</t>
+  </si>
+  <si>
+    <t>serotype_14</t>
+  </si>
+  <si>
+    <t>serotype_15</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>6A/6B</t>
+  </si>
+  <si>
+    <t>6A_6B_6C_6D</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>06A</t>
+  </si>
+  <si>
+    <t>06B</t>
+  </si>
+  <si>
+    <t>06C</t>
+  </si>
+  <si>
+    <t>06D</t>
+  </si>
+  <si>
+    <t>06E</t>
+  </si>
+  <si>
+    <t>06A-I</t>
+  </si>
+  <si>
+    <t>06A-II</t>
+  </si>
+  <si>
+    <t>06A-III</t>
+  </si>
+  <si>
+    <t>06A-IV</t>
+  </si>
+  <si>
+    <t>06A-V</t>
+  </si>
+  <si>
+    <t>06A-VI</t>
+  </si>
+  <si>
+    <t>06B-I</t>
+  </si>
+  <si>
+    <t>06B-II</t>
+  </si>
+  <si>
+    <t>06B-III</t>
+  </si>
+  <si>
+    <t>06C-I</t>
+  </si>
+  <si>
+    <t>6C/6D</t>
+  </si>
+  <si>
+    <t>Serogroup_6_(6E)</t>
+  </si>
+  <si>
+    <t>7F/7A</t>
+  </si>
+  <si>
+    <t>07F</t>
+  </si>
+  <si>
+    <t>07A</t>
+  </si>
+  <si>
+    <t>7B/40</t>
+  </si>
+  <si>
+    <t>07B</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>07C</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>9A/9V</t>
+  </si>
+  <si>
+    <t>09V</t>
+  </si>
+  <si>
+    <t>09A</t>
+  </si>
+  <si>
+    <t>9N/9L</t>
+  </si>
+  <si>
+    <t>09N</t>
+  </si>
+  <si>
+    <t>09L</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>10B</t>
+  </si>
+  <si>
+    <t>10C</t>
+  </si>
+  <si>
+    <t>10F</t>
+  </si>
+  <si>
+    <t>11F</t>
+  </si>
+  <si>
+    <t>11A/11D</t>
+  </si>
+  <si>
+    <t>11A</t>
+  </si>
+  <si>
+    <t>11D</t>
+  </si>
+  <si>
+    <t>11B/11C</t>
+  </si>
+  <si>
+    <t>11B</t>
+  </si>
+  <si>
+    <t>11C</t>
+  </si>
+  <si>
+    <t>12F</t>
+  </si>
+  <si>
+    <t>12F_12A_12B_44_46</t>
+  </si>
+  <si>
+    <t>12A</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>12A/12B/44/46</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15F</t>
+  </si>
+  <si>
+    <t>15F_15A</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>15B/15C</t>
+  </si>
+  <si>
+    <t>15B</t>
+  </si>
+  <si>
+    <t>15C</t>
+  </si>
+  <si>
+    <t>16A</t>
+  </si>
+  <si>
+    <t>16F</t>
+  </si>
+  <si>
+    <t>17A</t>
+  </si>
+  <si>
+    <t>17F</t>
+  </si>
+  <si>
+    <t>18A</t>
+  </si>
+  <si>
+    <t>18C/18B</t>
+  </si>
+  <si>
+    <t>18C</t>
+  </si>
+  <si>
+    <t>18B</t>
+  </si>
+  <si>
+    <t>18F</t>
+  </si>
+  <si>
+    <t>19A</t>
+  </si>
+  <si>
+    <t>19A_19AF</t>
+  </si>
+  <si>
+    <t>19A-I</t>
+  </si>
+  <si>
+    <t>19A-II</t>
+  </si>
+  <si>
+    <t>19A-III</t>
+  </si>
+  <si>
+    <t>19AF</t>
+  </si>
+  <si>
+    <t>19F</t>
+  </si>
+  <si>
+    <t>19F-I</t>
+  </si>
+  <si>
+    <t>19F-II</t>
+  </si>
+  <si>
+    <t>19F-III</t>
+  </si>
+  <si>
+    <t>19F-IV</t>
+  </si>
+  <si>
+    <t>19B</t>
+  </si>
+  <si>
+    <t>19C</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22A</t>
+  </si>
+  <si>
+    <t>22F</t>
+  </si>
+  <si>
+    <t>23A</t>
+  </si>
+  <si>
+    <t>23B</t>
+  </si>
+  <si>
+    <t>23B1</t>
+  </si>
+  <si>
+    <t>23F</t>
+  </si>
+  <si>
+    <t>24F/24B</t>
+  </si>
+  <si>
+    <t>24F</t>
+  </si>
+  <si>
+    <t>24B</t>
+  </si>
+  <si>
+    <t>24F2</t>
+  </si>
+  <si>
+    <t>24A</t>
+  </si>
+  <si>
+    <t>25F/25A</t>
+  </si>
+  <si>
+    <t>25F_25A_38</t>
+  </si>
+  <si>
+    <t>25F</t>
+  </si>
+  <si>
+    <t>25A</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28F/28A</t>
+  </si>
+  <si>
+    <t>28F</t>
+  </si>
+  <si>
+    <t>28A</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32F/32A</t>
+  </si>
+  <si>
+    <t>32F</t>
+  </si>
+  <si>
+    <t>32A</t>
+  </si>
+  <si>
+    <t>33F/33A</t>
+  </si>
+  <si>
+    <t>33F</t>
+  </si>
+  <si>
+    <t>33A</t>
+  </si>
+  <si>
+    <t>33F2</t>
+  </si>
+  <si>
+    <t>33B</t>
+  </si>
+  <si>
+    <t>33C</t>
+  </si>
+  <si>
+    <t>33D</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35B/35D</t>
+  </si>
+  <si>
+    <t>35B</t>
+  </si>
+  <si>
+    <t>35A/35C/42</t>
+  </si>
+  <si>
+    <t>35C</t>
+  </si>
+  <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>35F</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>41A</t>
+  </si>
+  <si>
+    <t>41F</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>47A</t>
+  </si>
+  <si>
+    <t>47F</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>var_type</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>variant</t>
+  </si>
+  <si>
+    <t>allele</t>
+  </si>
+  <si>
+    <t>wciN</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>wciI</t>
+  </si>
+  <si>
+    <t>gene_presence</t>
+  </si>
+  <si>
+    <t>glf</t>
+  </si>
+  <si>
+    <t>detected</t>
+  </si>
+  <si>
+    <t>rmlB</t>
+  </si>
+  <si>
+    <t>rmlD</t>
+  </si>
+  <si>
+    <t>wcjE</t>
+  </si>
+  <si>
+    <t>not_detected</t>
+  </si>
+  <si>
+    <t>wzy</t>
+  </si>
+  <si>
+    <t>wcyD</t>
+  </si>
+  <si>
+    <t>wcyV</t>
+  </si>
+  <si>
+    <t>group_name</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>non-encapsulated</t>
+  </si>
+  <si>
+    <t>NT3b</t>
+  </si>
+  <si>
+    <t>NT2</t>
+  </si>
+  <si>
+    <t>NT3b1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="167" formatCode="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -648,22 +660,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -671,18 +668,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -695,7 +690,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -703,142 +698,436 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2050" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0536306F-3A0D-A25C-EF63-8CB92E9D7F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:R77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R65" sqref="R65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="2" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.53"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="4" max="17" width="9.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="2" customWidth="1"/>
+    <col min="19" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -894,7 +1183,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -905,7 +1194,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -916,7 +1205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -927,7 +1216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -938,7 +1227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -949,7 +1238,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
@@ -1005,7 +1294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
@@ -1061,7 +1350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>48</v>
       </c>
@@ -1117,7 +1406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
@@ -1131,7 +1420,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>52</v>
       </c>
@@ -1145,7 +1434,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1156,7 +1445,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -1167,7 +1456,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>59</v>
       </c>
@@ -1181,7 +1470,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>62</v>
       </c>
@@ -1195,7 +1484,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -1206,7 +1495,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
@@ -1217,7 +1506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>67</v>
       </c>
@@ -1228,7 +1517,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>68</v>
       </c>
@@ -1239,7 +1528,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -1250,7 +1539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>70</v>
       </c>
@@ -1278,7 +1567,7 @@
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>73</v>
       </c>
@@ -1292,7 +1581,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -1318,7 +1607,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>82</v>
       </c>
@@ -1344,7 +1633,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>83</v>
       </c>
@@ -1355,7 +1644,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -1366,7 +1655,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>85</v>
       </c>
@@ -1383,7 +1672,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>87</v>
       </c>
@@ -1400,7 +1689,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -1414,7 +1703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>91</v>
       </c>
@@ -1425,7 +1714,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>92</v>
       </c>
@@ -1436,7 +1725,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -1447,7 +1736,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
@@ -1458,7 +1747,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -1469,7 +1758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
@@ -1483,7 +1772,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -1497,7 +1786,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
@@ -1508,7 +1797,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>100</v>
       </c>
@@ -1534,7 +1823,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
@@ -1560,7 +1849,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>106</v>
       </c>
@@ -1583,7 +1872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>111</v>
       </c>
@@ -1594,7 +1883,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>112</v>
       </c>
@@ -1605,7 +1894,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -1616,7 +1905,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>114</v>
       </c>
@@ -1627,7 +1916,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
@@ -1638,7 +1927,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>116</v>
       </c>
@@ -1649,7 +1938,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>117</v>
       </c>
@@ -1660,7 +1949,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>118</v>
       </c>
@@ -1674,7 +1963,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>120</v>
       </c>
@@ -1685,7 +1974,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>121</v>
       </c>
@@ -1702,7 +1991,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>125</v>
       </c>
@@ -1713,7 +2002,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>126</v>
       </c>
@@ -1730,7 +2019,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>130</v>
       </c>
@@ -1741,7 +2030,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>131</v>
       </c>
@@ -1755,7 +2044,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>134</v>
       </c>
@@ -1766,7 +2055,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>135</v>
       </c>
@@ -1777,7 +2066,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>136</v>
       </c>
@@ -1791,7 +2080,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>139</v>
       </c>
@@ -1807,9 +2096,9 @@
       <c r="F58" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -1820,7 +2109,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -1831,7 +2120,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -1842,7 +2131,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>146</v>
       </c>
@@ -1853,7 +2142,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>147</v>
       </c>
@@ -1864,7 +2153,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>149</v>
       </c>
@@ -1881,7 +2170,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>153</v>
       </c>
@@ -1892,7 +2181,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -1903,7 +2192,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>155</v>
       </c>
@@ -1914,7 +2203,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>156</v>
       </c>
@@ -1934,7 +2223,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>157</v>
       </c>
@@ -1944,10 +2233,10 @@
       <c r="D69" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E69" s="0"/>
-      <c r="F69" s="0"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69"/>
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -1957,9 +2246,9 @@
       <c r="D70" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>158</v>
       </c>
@@ -1970,7 +2259,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>159</v>
       </c>
@@ -1981,7 +2270,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -1992,7 +2281,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>161</v>
       </c>
@@ -2003,7 +2292,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>162</v>
       </c>
@@ -2014,7 +2303,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
@@ -2025,7 +2314,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>164</v>
       </c>
@@ -2036,120 +2325,128 @@
         <v>164</v>
       </c>
     </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R77"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:R77" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="21.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="9" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="16.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="24.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="9" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="9" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="9" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="9" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="9" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="9" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="9" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="9" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="9" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="9" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="9" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="9" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="9" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="9" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="9" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="9" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="9" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="9" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="9" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="85" style="9" width="9.14"/>
+    <col min="1" max="1" width="21.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="9" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" style="9" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="9" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="9" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="9" customWidth="1"/>
+    <col min="19" max="19" width="21" style="9" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" style="9" customWidth="1"/>
+    <col min="21" max="21" width="21" style="9" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" style="9" customWidth="1"/>
+    <col min="23" max="23" width="21" style="9" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" style="9" customWidth="1"/>
+    <col min="25" max="25" width="21" style="9" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" style="9" customWidth="1"/>
+    <col min="27" max="27" width="21" style="9" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" style="9" customWidth="1"/>
+    <col min="29" max="29" width="21" style="9" customWidth="1"/>
+    <col min="30" max="30" width="17.5703125" style="9" customWidth="1"/>
+    <col min="31" max="31" width="22.28515625" style="9" customWidth="1"/>
+    <col min="32" max="32" width="21" style="9" customWidth="1"/>
+    <col min="33" max="33" width="22.28515625" style="9" customWidth="1"/>
+    <col min="34" max="34" width="21" style="9" customWidth="1"/>
+    <col min="35" max="35" width="22.28515625" style="9" customWidth="1"/>
+    <col min="36" max="36" width="21" style="9" customWidth="1"/>
+    <col min="37" max="37" width="23.28515625" style="9" customWidth="1"/>
+    <col min="38" max="38" width="22.140625" style="9" customWidth="1"/>
+    <col min="39" max="39" width="23.28515625" style="9" customWidth="1"/>
+    <col min="40" max="40" width="22.140625" style="9" customWidth="1"/>
+    <col min="41" max="41" width="23.28515625" style="9" customWidth="1"/>
+    <col min="42" max="42" width="22.140625" style="9" customWidth="1"/>
+    <col min="43" max="43" width="18.5703125" style="9" customWidth="1"/>
+    <col min="44" max="44" width="23.28515625" style="9" customWidth="1"/>
+    <col min="45" max="45" width="22.140625" style="9" customWidth="1"/>
+    <col min="46" max="46" width="23.28515625" style="9" customWidth="1"/>
+    <col min="47" max="47" width="22.140625" style="9" customWidth="1"/>
+    <col min="48" max="48" width="23.28515625" style="9" customWidth="1"/>
+    <col min="49" max="49" width="22.140625" style="9" customWidth="1"/>
+    <col min="50" max="50" width="23.28515625" style="9" customWidth="1"/>
+    <col min="51" max="51" width="22.140625" style="9" customWidth="1"/>
+    <col min="52" max="52" width="23.28515625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="22.140625" style="9" customWidth="1"/>
+    <col min="54" max="54" width="23.28515625" style="9" customWidth="1"/>
+    <col min="55" max="55" width="22.140625" style="9" customWidth="1"/>
+    <col min="56" max="56" width="23.28515625" style="9" customWidth="1"/>
+    <col min="57" max="57" width="22.140625" style="9" customWidth="1"/>
+    <col min="58" max="58" width="11.5703125" style="9" customWidth="1"/>
+    <col min="59" max="59" width="22.28515625" style="9" customWidth="1"/>
+    <col min="60" max="60" width="21" style="9" customWidth="1"/>
+    <col min="61" max="61" width="22.28515625" style="9" customWidth="1"/>
+    <col min="62" max="62" width="21" style="9" customWidth="1"/>
+    <col min="63" max="63" width="22.28515625" style="9" customWidth="1"/>
+    <col min="64" max="64" width="21" style="9" customWidth="1"/>
+    <col min="65" max="65" width="22.28515625" style="9" customWidth="1"/>
+    <col min="66" max="66" width="21" style="9" customWidth="1"/>
+    <col min="67" max="67" width="22.28515625" style="9" customWidth="1"/>
+    <col min="68" max="68" width="21" style="9" customWidth="1"/>
+    <col min="69" max="69" width="22.28515625" style="9" customWidth="1"/>
+    <col min="70" max="70" width="21" style="9" customWidth="1"/>
+    <col min="71" max="71" width="22.28515625" style="9" customWidth="1"/>
+    <col min="72" max="72" width="21" style="9" customWidth="1"/>
+    <col min="73" max="73" width="11.5703125" style="9" customWidth="1"/>
+    <col min="74" max="74" width="22.28515625" style="9" customWidth="1"/>
+    <col min="75" max="75" width="21" style="9" customWidth="1"/>
+    <col min="76" max="76" width="22.28515625" style="9" customWidth="1"/>
+    <col min="77" max="77" width="21" style="9" customWidth="1"/>
+    <col min="78" max="78" width="22.28515625" style="9" customWidth="1"/>
+    <col min="79" max="79" width="21" style="9" customWidth="1"/>
+    <col min="80" max="80" width="22.28515625" style="9" customWidth="1"/>
+    <col min="81" max="81" width="21" style="9" customWidth="1"/>
+    <col min="82" max="82" width="11.5703125" style="9" customWidth="1"/>
+    <col min="83" max="83" width="22.28515625" style="9" customWidth="1"/>
+    <col min="84" max="84" width="21" style="9" customWidth="1"/>
+    <col min="85" max="1025" width="9.140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2166,7 +2463,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
@@ -2180,7 +2477,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>47</v>
       </c>
@@ -2194,7 +2491,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>48</v>
       </c>
@@ -2208,7 +2505,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>76</v>
       </c>
@@ -2222,7 +2519,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>82</v>
       </c>
@@ -2236,7 +2533,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>85</v>
       </c>
@@ -2250,7 +2547,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>85</v>
       </c>
@@ -2264,7 +2561,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>85</v>
       </c>
@@ -2278,7 +2575,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>85</v>
       </c>
@@ -2292,7 +2589,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>87</v>
       </c>
@@ -2306,7 +2603,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>87</v>
       </c>
@@ -2320,7 +2617,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>87</v>
       </c>
@@ -2334,7 +2631,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
@@ -2348,7 +2645,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>100</v>
       </c>
@@ -2362,7 +2659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>106</v>
       </c>
@@ -2376,7 +2673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>126</v>
       </c>
@@ -2390,7 +2687,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>126</v>
       </c>
@@ -2404,7 +2701,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>156</v>
       </c>
@@ -2418,7 +2715,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>156</v>
       </c>
@@ -2432,121 +2729,96 @@
         <v>177</v>
       </c>
     </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E21"/>
+  <autoFilter ref="A1:E21" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1:D20" type="whole">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D20" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="7" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="7" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="7" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="7" width="9.14"/>
+    <col min="1" max="1" width="14.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14" style="7" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="7" customWidth="1"/>
+    <col min="10" max="13" width="11.28515625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="7" customWidth="1"/>
+    <col min="16" max="1025" width="9.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>165</v>
       </c>
@@ -2563,7 +2835,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>169</v>
       </c>
@@ -2578,7 +2850,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>169</v>
       </c>
@@ -2593,7 +2865,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>169</v>
       </c>
@@ -2608,7 +2880,7 @@
       </c>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>169</v>
       </c>
@@ -2623,7 +2895,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>169</v>
       </c>
@@ -2638,7 +2910,7 @@
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>169</v>
       </c>
@@ -2653,7 +2925,7 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
@@ -2668,7 +2940,7 @@
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>169</v>
       </c>
@@ -2683,7 +2955,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>169</v>
       </c>
@@ -2698,7 +2970,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>175</v>
       </c>
@@ -2713,7 +2985,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>175</v>
       </c>
@@ -2728,7 +3000,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>175</v>
       </c>
@@ -2743,7 +3015,7 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>175</v>
       </c>
@@ -2758,7 +3030,7 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>175</v>
       </c>
@@ -2773,7 +3045,7 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>175</v>
       </c>
@@ -2788,7 +3060,7 @@
       </c>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>175</v>
       </c>
@@ -2803,7 +3075,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>175</v>
       </c>
@@ -2818,7 +3090,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>175</v>
       </c>
@@ -2834,7 +3106,7 @@
       <c r="F19" s="9"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>175</v>
       </c>
@@ -2850,20 +3122,14 @@
       <c r="H20" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20"/>
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19:C20" type="whole">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C20" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added extra references for non-typeables to CTVdb
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\PycharmProjects\PneumoKITy\Database_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651B090A-9632-46E9-AEB4-B7B583DE2983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A252E00F-2C51-416F-9682-99D9C4FA3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="199">
   <si>
     <t>predicted_pheno</t>
   </si>
@@ -642,6 +642,30 @@
   </si>
   <si>
     <t>NT3b1</t>
+  </si>
+  <si>
+    <t>NT2-1</t>
+  </si>
+  <si>
+    <t>NT2-2</t>
+  </si>
+  <si>
+    <t>NT3</t>
+  </si>
+  <si>
+    <t>NT3-1</t>
+  </si>
+  <si>
+    <t>NT3-2</t>
+  </si>
+  <si>
+    <t>NT3-3</t>
+  </si>
+  <si>
+    <t>NT3-4</t>
+  </si>
+  <si>
+    <t>NT3-5</t>
   </si>
 </sst>
 </file>
@@ -651,7 +675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -678,6 +702,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1113,8 +1143,8 @@
   <dimension ref="A1:R78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R65" sqref="R65"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2200,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>153</v>
       </c>
@@ -2181,7 +2211,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -2192,7 +2222,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>155</v>
       </c>
@@ -2203,7 +2233,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>156</v>
       </c>
@@ -2223,7 +2253,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>157</v>
       </c>
@@ -2236,7 +2266,7 @@
       <c r="E69"/>
       <c r="F69"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -2248,7 +2278,7 @@
       </c>
       <c r="F70"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>158</v>
       </c>
@@ -2259,7 +2289,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>159</v>
       </c>
@@ -2270,7 +2300,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -2281,7 +2311,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>161</v>
       </c>
@@ -2292,7 +2322,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>162</v>
       </c>
@@ -2303,7 +2333,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
@@ -2314,7 +2344,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>164</v>
       </c>
@@ -2325,7 +2355,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>187</v>
       </c>
@@ -2336,14 +2366,39 @@
         <v>188</v>
       </c>
       <c r="E78" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>190</v>
+      <c r="G78" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="L78" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="N78" s="2" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:R77" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
fix missing NT-3 in database
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\PycharmProjects\PneumoKITy\Database_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A252E00F-2C51-416F-9682-99D9C4FA3F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E609297F-0167-4E63-A96F-360733AA68CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="200">
   <si>
     <t>predicted_pheno</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>NT3-5</t>
+  </si>
+  <si>
+    <t>NT2-3</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G90" sqref="G90"/>
+      <selection pane="bottomLeft" activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,7 +2203,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>153</v>
       </c>
@@ -2211,7 +2214,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>155</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>156</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>157</v>
       </c>
@@ -2266,7 +2269,7 @@
       <c r="E69"/>
       <c r="F69"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -2278,7 +2281,7 @@
       </c>
       <c r="F70"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>158</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>159</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>160</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>161</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>162</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>163</v>
       </c>
@@ -2344,7 +2347,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>164</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>187</v>
       </c>
@@ -2378,21 +2381,24 @@
         <v>192</v>
       </c>
       <c r="I78" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J78" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="J78" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="M78" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="M78" s="2" t="s">
+      <c r="N78" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="N78" s="2" t="s">
+      <c r="O78" s="2" t="s">
         <v>198</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to add 36A and 36B
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\PycharmProjects\PneumoKITy_update\Database_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F2B0A9-B925-4C03-8ABF-040059FB4EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A36806B-CB17-4200-9AD3-EC6BC7A179EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Serotype" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="4. Variants" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Serotype'!$A$1:$R$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1. Serotype'!$A$1:$R$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. SerotypeVariants'!$A$1:$E$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4. Variants'!$A$1:$E$20</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="1">'2. SerotypeVariants'!$A$1:$E$20</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="190">
   <si>
     <t>predicted_pheno</t>
   </si>
@@ -530,9 +530,6 @@
     <t>35F</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>37</t>
   </si>
   <si>
@@ -636,6 +633,12 @@
   </si>
   <si>
     <t>15A/15D</t>
+  </si>
+  <si>
+    <t>36A</t>
+  </si>
+  <si>
+    <t>36B</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R77"/>
+  <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1663,7 +1666,7 @@
         <v>85</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>19</v>
@@ -1675,15 +1678,15 @@
         <v>85</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>19</v>
@@ -1695,7 +1698,7 @@
         <v>85</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
@@ -2192,150 +2195,161 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69"/>
-      <c r="F69"/>
+        <v>128</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E70"/>
       <c r="F70"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
-        <v>157</v>
+        <v>54</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>157</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F71"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R77" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:R78" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2443,16 +2457,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2460,13 +2474,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2474,13 +2488,13 @@
         <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2488,13 +2502,13 @@
         <v>48</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2502,10 +2516,10 @@
         <v>76</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>21</v>
@@ -2516,10 +2530,10 @@
         <v>82</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>18</v>
@@ -2530,13 +2544,13 @@
         <v>85</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2544,13 +2558,13 @@
         <v>85</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2558,13 +2572,13 @@
         <v>85</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2572,69 +2586,69 @@
         <v>85</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2642,10 +2656,10 @@
         <v>99</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>18</v>
@@ -2656,10 +2670,10 @@
         <v>105</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>21</v>
@@ -2670,13 +2684,13 @@
         <v>125</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2684,41 +2698,41 @@
         <v>125</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2752,7 +2766,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -2767,7 +2781,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -2790,7 +2804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -2812,30 +2826,30 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>167</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>170</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>30</v>
@@ -2844,13 +2858,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>30</v>
@@ -2859,13 +2873,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>30</v>
@@ -2874,10 +2888,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>18</v>
@@ -2889,10 +2903,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
@@ -2904,10 +2918,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>18</v>
@@ -2919,10 +2933,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>21</v>
@@ -2934,13 +2948,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>126</v>
@@ -2949,13 +2963,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>126</v>
@@ -2964,133 +2978,133 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>176</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>126</v>
@@ -3100,13 +3114,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Add 35D reference CPS to references.fasta/msh and stage 1 determination
</commit_message>
<xml_diff>
--- a/Database_tools/CTVdb_import_standard_template.xlsx
+++ b/Database_tools/CTVdb_import_standard_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carmen\PycharmProjects\PneumoKITy_update\Database_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A36806B-CB17-4200-9AD3-EC6BC7A179EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB06380-B539-4CA4-8DB6-51D11D58C406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="191">
   <si>
     <t>predicted_pheno</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>36B</t>
+  </si>
+  <si>
+    <t>35D</t>
   </si>
 </sst>
 </file>
@@ -1119,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2163,6 +2166,9 @@
       </c>
       <c r="D63" s="2" t="s">
         <v>147</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>